<commit_message>
dodajanje k analizi, sledi napoved
</commit_message>
<xml_diff>
--- a/Diploma podatki/ANALIZA_POSLOVANJA.xlsx
+++ b/Diploma podatki/ANALIZA_POSLOVANJA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neža\Documents\GitHub\Diplomska-naloga-\Diploma podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D44FA4-7CCE-41A1-AAD8-7187160F329F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9628F-340F-4067-BFF2-D1F3B6985DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="11" activeTab="14" xr2:uid="{0DAC0375-5244-478E-9483-C7B8579F68F1}"/>
   </bookViews>
@@ -639,8 +639,71 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neža</author>
+  </authors>
+  <commentList>
+    <comment ref="A88" authorId="0" shapeId="0" xr:uid="{6DF1250F-C2CC-461E-B380-7016B7F385BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Neža:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+po vzoru študije številka 2
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B89" authorId="0" shapeId="0" xr:uid="{4136F1E8-28B4-4A5F-AC27-63E7CEFEEE0F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Neža:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+povprečje 5 let</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="331">
   <si>
     <t>opredmetena osnovna</t>
   </si>
@@ -1604,6 +1667,36 @@
   <si>
     <t>čisti dobiček/prihodki od prodaje</t>
   </si>
+  <si>
+    <t>Delež delnic, v lasti drugih delničarjev, ne podjetja</t>
+  </si>
+  <si>
+    <t>KAZALCI ZA ODBITEK ZARADI POMANJKANJA TRŽLJIVOSTI</t>
+  </si>
+  <si>
+    <t>total assets</t>
+  </si>
+  <si>
+    <t>book value of equity</t>
+  </si>
+  <si>
+    <t>net income</t>
+  </si>
+  <si>
+    <t>net profit margin</t>
+  </si>
+  <si>
+    <t>market cap</t>
+  </si>
+  <si>
+    <t>Dolžniško financiranje</t>
+  </si>
+  <si>
+    <t>lastniško financiranje</t>
+  </si>
+  <si>
+    <t>neto dolg/EBITDA</t>
+  </si>
 </sst>
 </file>
 
@@ -1619,7 +1712,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1788,6 +1881,21 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1851,7 +1959,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -2616,6 +2724,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2629,7 +2750,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="559">
+  <cellXfs count="567">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -3049,8 +3170,6 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -3138,8 +3257,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -3174,6 +3291,17 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="8" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3198,13 +3326,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="8" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hiperpovezava" xfId="9" builtinId="8"/>
@@ -3373,7 +3506,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'ANALIZA DELNICE'!$C$13:$G$13</c:f>
+              <c:f>'ANALIZA DELNICE'!$C$14:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3397,7 +3530,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ANALIZA DELNICE'!$C$14:$G$14</c:f>
+              <c:f>'ANALIZA DELNICE'!$C$15:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3473,7 +3606,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'ANALIZA DELNICE'!$C$13:$G$13</c15:sqref>
+                          <c15:sqref>'ANALIZA DELNICE'!$C$14:$G$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3503,7 +3636,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'ANALIZA DELNICE'!$C$14:$G$14</c15:sqref>
+                          <c15:sqref>'ANALIZA DELNICE'!$C$15:$G$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12580,7 +12713,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$A$54</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$A$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12615,7 +12748,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$53:$F$53</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$54:$F$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -12639,7 +12772,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$55:$F$55</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$56:$F$56</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -12673,7 +12806,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$A$57</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12708,7 +12841,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$53:$F$53</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$54:$F$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -12732,7 +12865,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$58:$F$58</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$59:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13159,7 +13292,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$A$35</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13194,7 +13327,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$34:$F$34</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$35:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13218,7 +13351,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$36:$F$36</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$37:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13252,7 +13385,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$A$38</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13287,7 +13420,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$39:$F$39</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13321,7 +13454,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$A$41</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13356,7 +13489,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$42:$F$42</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$43:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13795,7 +13928,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$A$71</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$A$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13816,7 +13949,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$68:$F$68</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$69:$F$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13840,7 +13973,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$71:$F$71</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$72:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -17094,7 +17227,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'KAZALNIKI - PODJETJE X'!$B$58:$F$58</c:f>
+              <c:f>'KAZALNIKI - PODJETJE X'!$B$59:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -30604,7 +30737,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31238,7 +31371,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31270,13 +31403,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>64770</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31308,13 +31441,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31352,7 +31485,7 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31384,13 +31517,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31422,13 +31555,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31460,13 +31593,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -32247,7 +32380,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32704,7 +32837,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F18" s="29"/>
-      <c r="G18" s="461"/>
+      <c r="G18" s="459"/>
     </row>
     <row r="19" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="193" t="s">
@@ -32790,43 +32923,43 @@
       <c r="A21" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="435">
+      <c r="B21" s="433">
         <f>B20/'PRIHODKI IN STROŠKI'!B$6</f>
         <v>0.18794790395802333</v>
       </c>
-      <c r="C21" s="435">
+      <c r="C21" s="433">
         <f>C20/'PRIHODKI IN STROŠKI'!C$6</f>
         <v>0.20842355143456792</v>
       </c>
-      <c r="D21" s="435">
+      <c r="D21" s="433">
         <f>D20/'PRIHODKI IN STROŠKI'!D$6</f>
         <v>0.17662969259205374</v>
       </c>
-      <c r="E21" s="435">
+      <c r="E21" s="433">
         <f>E20/'PRIHODKI IN STROŠKI'!E$6</f>
         <v>0.15445327243300794</v>
       </c>
-      <c r="F21" s="436">
+      <c r="F21" s="434">
         <f>F20/'PRIHODKI IN STROŠKI'!F$6</f>
         <v>0.15592942626780612</v>
       </c>
-      <c r="G21" s="437">
+      <c r="G21" s="435">
         <f>G20/'PRIHODKI IN STROŠKI'!G$6</f>
         <v>0.15000000000000005</v>
       </c>
-      <c r="H21" s="435">
+      <c r="H21" s="433">
         <f>H20/'PRIHODKI IN STROŠKI'!H$6</f>
         <v>0.12000000000000005</v>
       </c>
-      <c r="I21" s="435">
+      <c r="I21" s="433">
         <f>I20/'PRIHODKI IN STROŠKI'!I$6</f>
         <v>0.12999999999999998</v>
       </c>
-      <c r="J21" s="435">
+      <c r="J21" s="433">
         <f>J20/'PRIHODKI IN STROŠKI'!J$6</f>
         <v>0.13</v>
       </c>
-      <c r="K21" s="438">
+      <c r="K21" s="436">
         <f>K20/'PRIHODKI IN STROŠKI'!K$6</f>
         <v>0.12000000000000001</v>
       </c>
@@ -32835,7 +32968,7 @@
       <c r="A22" s="285" t="s">
         <v>224</v>
       </c>
-      <c r="B22" s="439"/>
+      <c r="B22" s="437"/>
       <c r="C22" s="361">
         <f>C20-B20</f>
         <v>3685368</v>
@@ -32880,7 +33013,7 @@
       <c r="F24" s="29"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="434"/>
+      <c r="B25" s="432"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32895,7 +33028,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33985,7 +34118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5B39DD-43BF-4414-9258-52BD9D95E4C8}">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -34092,7 +34225,7 @@
       <c r="I4" s="240"/>
       <c r="J4" s="240"/>
       <c r="K4" s="240"/>
-      <c r="L4" s="463"/>
+      <c r="L4" s="461"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="250" t="s">
@@ -34188,7 +34321,7 @@
       <c r="I8" s="240"/>
       <c r="J8" s="240"/>
       <c r="K8" s="240"/>
-      <c r="L8" s="463"/>
+      <c r="L8" s="461"/>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="302" t="s">
@@ -34675,7 +34808,7 @@
         <f>K24</f>
         <v>180115.56</v>
       </c>
-      <c r="L26" s="434"/>
+      <c r="L26" s="432"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="84" t="s">
@@ -34709,7 +34842,7 @@
         <f t="shared" si="7"/>
         <v>6078411.595999999</v>
       </c>
-      <c r="L27" s="434"/>
+      <c r="L27" s="432"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
@@ -34725,7 +34858,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="52"/>
-      <c r="L28" s="434"/>
+      <c r="L28" s="432"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="86" t="s">
@@ -36218,8 +36351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0E449A-96AB-4A84-BE80-DE3A976793FE}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37901,8 +38034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCCC69F-E9DD-4E05-8C72-E6D15378301D}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37939,7 +38072,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="422" t="s">
+      <c r="A5" s="420" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="100">
@@ -37959,7 +38092,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="425" t="s">
+      <c r="A6" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B6" s="216"/>
@@ -37981,7 +38114,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="431" t="s">
+      <c r="A7" s="429" t="s">
         <v>176</v>
       </c>
       <c r="B7" s="100">
@@ -38001,7 +38134,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="425" t="s">
+      <c r="A8" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B8" s="216"/>
@@ -38023,7 +38156,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="422" t="s">
+      <c r="A9" s="420" t="s">
         <v>177</v>
       </c>
       <c r="B9" s="100">
@@ -38043,7 +38176,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="425" t="s">
+      <c r="A10" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B10" s="216"/>
@@ -38065,7 +38198,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" s="160" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="432" t="s">
+      <c r="A11" s="430" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="236">
@@ -38090,7 +38223,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="422" t="s">
+      <c r="A12" s="420" t="s">
         <v>179</v>
       </c>
       <c r="B12" s="100">
@@ -38110,7 +38243,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="425" t="s">
+      <c r="A13" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B13" s="216"/>
@@ -38132,7 +38265,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="422" t="s">
+      <c r="A14" s="420" t="s">
         <v>180</v>
       </c>
       <c r="B14" s="100">
@@ -38152,7 +38285,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="422" t="s">
+      <c r="A15" s="420" t="s">
         <v>169</v>
       </c>
       <c r="B15" s="100">
@@ -38185,7 +38318,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="422" t="s">
+      <c r="A17" s="420" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="100">
@@ -38205,7 +38338,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="425" t="s">
+      <c r="A18" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B18" s="216"/>
@@ -38227,7 +38360,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="431" t="s">
+      <c r="A19" s="429" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="100">
@@ -38247,7 +38380,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="425" t="s">
+      <c r="A20" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B20" s="216"/>
@@ -38269,7 +38402,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="422" t="s">
+      <c r="A21" s="420" t="s">
         <v>177</v>
       </c>
       <c r="B21" s="100">
@@ -38294,7 +38427,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="425" t="s">
+      <c r="A22" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B22" s="216"/>
@@ -38316,7 +38449,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" s="160" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="432" t="s">
+      <c r="A23" s="430" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="236">
@@ -38341,7 +38474,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="422" t="s">
+      <c r="A24" s="420" t="s">
         <v>182</v>
       </c>
       <c r="B24" s="100">
@@ -38361,7 +38494,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="425" t="s">
+      <c r="A25" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B25" s="216"/>
@@ -38383,7 +38516,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="422" t="s">
+      <c r="A26" s="420" t="s">
         <v>169</v>
       </c>
       <c r="B26" s="100">
@@ -38416,7 +38549,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="422" t="s">
+      <c r="A28" s="420" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="100">
@@ -38436,7 +38569,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="425" t="s">
+      <c r="A29" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B29" s="216"/>
@@ -38458,7 +38591,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="431" t="s">
+      <c r="A30" s="429" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="100">
@@ -38478,7 +38611,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="425" t="s">
+      <c r="A31" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B31" s="216"/>
@@ -38500,7 +38633,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="422" t="s">
+      <c r="A32" s="420" t="s">
         <v>177</v>
       </c>
       <c r="B32" s="100">
@@ -38525,7 +38658,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="425" t="s">
+      <c r="A33" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B33" s="216"/>
@@ -38547,7 +38680,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="432" t="s">
+      <c r="A34" s="430" t="s">
         <v>178</v>
       </c>
       <c r="B34" s="236">
@@ -38572,7 +38705,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="422" t="s">
+      <c r="A35" s="420" t="s">
         <v>179</v>
       </c>
       <c r="B35" s="100">
@@ -38592,7 +38725,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="425" t="s">
+      <c r="A36" s="423" t="s">
         <v>175</v>
       </c>
       <c r="B36" s="216"/>
@@ -38614,7 +38747,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="422" t="s">
+      <c r="A37" s="420" t="s">
         <v>169</v>
       </c>
       <c r="B37" s="100">
@@ -38647,7 +38780,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="422" t="s">
+      <c r="A39" s="420" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="100">
@@ -38672,7 +38805,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="433" t="s">
+      <c r="A40" s="431" t="s">
         <v>184</v>
       </c>
       <c r="B40" s="240"/>
@@ -38694,32 +38827,32 @@
       </c>
     </row>
     <row r="41" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="554" t="s">
+      <c r="A41" s="542" t="s">
         <v>318</v>
       </c>
-      <c r="B41" s="555">
+      <c r="B41" s="543">
         <f>'FCF - KONČNI_IZRAČUN'!B5</f>
         <v>2885192</v>
       </c>
-      <c r="C41" s="555">
+      <c r="C41" s="543">
         <f>'FCF - KONČNI_IZRAČUN'!C5</f>
         <v>6276734</v>
       </c>
-      <c r="D41" s="555">
+      <c r="D41" s="543">
         <f>'FCF - KONČNI_IZRAČUN'!D5</f>
         <v>8390559</v>
       </c>
-      <c r="E41" s="555">
+      <c r="E41" s="543">
         <f>'FCF - KONČNI_IZRAČUN'!E5</f>
         <v>10217587</v>
       </c>
-      <c r="F41" s="556">
+      <c r="F41" s="544">
         <f>'FCF - KONČNI_IZRAČUN'!F5</f>
         <v>10844757</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="427" t="s">
+      <c r="A42" s="425" t="s">
         <v>185</v>
       </c>
       <c r="B42" s="242">
@@ -38744,7 +38877,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="425" t="s">
+      <c r="A43" s="423" t="s">
         <v>186</v>
       </c>
       <c r="B43" s="216"/>
@@ -38766,7 +38899,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="422" t="s">
+      <c r="A44" s="420" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="100">
@@ -38791,7 +38924,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="422" t="s">
+      <c r="A45" s="420" t="s">
         <v>169</v>
       </c>
       <c r="B45" s="100">
@@ -38804,7 +38937,7 @@
       <c r="F45" s="211"/>
     </row>
     <row r="46" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="426" t="s">
+      <c r="A46" s="424" t="s">
         <v>187</v>
       </c>
       <c r="B46" s="218"/>
@@ -38947,7 +39080,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="557">
+      <c r="B55" s="545">
         <f>AVERAGE(B54:F54)</f>
         <v>0.1015751990728178</v>
       </c>
@@ -38960,22 +39093,23 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523C1896-62AA-4E45-8BD7-018962592130}">
-  <dimension ref="A1:F81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523C1896-62AA-4E45-8BD7-018962592130}">
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.21875" customWidth="1"/>
-    <col min="2" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="429" t="s">
+      <c r="A2" s="427" t="s">
         <v>134</v>
       </c>
       <c r="B2" s="209">
@@ -38995,7 +39129,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="422" t="s">
+      <c r="A3" s="420" t="s">
         <v>135</v>
       </c>
       <c r="B3" s="100">
@@ -39020,7 +39154,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="422" t="s">
+      <c r="A4" s="420" t="s">
         <v>136</v>
       </c>
       <c r="B4" s="100">
@@ -39045,7 +39179,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="422" t="s">
+      <c r="A5" s="420" t="s">
         <v>137</v>
       </c>
       <c r="B5" s="100">
@@ -39070,7 +39204,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="422" t="s">
+      <c r="A6" s="420" t="s">
         <v>138</v>
       </c>
       <c r="B6" s="100">
@@ -39095,7 +39229,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="423" t="s">
+      <c r="A7" s="421" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="212">
@@ -39116,7 +39250,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="429" t="s">
+      <c r="A10" s="427" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="209">
@@ -39136,7 +39270,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="422" t="s">
+      <c r="A11" s="420" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="100">
@@ -39161,7 +39295,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="422" t="s">
+      <c r="A12" s="420" t="s">
         <v>137</v>
       </c>
       <c r="B12" s="100">
@@ -39186,7 +39320,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="422" t="s">
+      <c r="A13" s="420" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="100">
@@ -39211,7 +39345,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="422" t="s">
+      <c r="A14" s="420" t="s">
         <v>142</v>
       </c>
       <c r="B14" s="100">
@@ -39234,7 +39368,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="423" t="s">
+      <c r="A15" s="421" t="s">
         <v>143</v>
       </c>
       <c r="B15" s="212">
@@ -39260,7 +39394,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="429" t="s">
+      <c r="A20" s="427" t="s">
         <v>144</v>
       </c>
       <c r="B20" s="209">
@@ -39280,7 +39414,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="422" t="s">
+      <c r="A21" s="420" t="s">
         <v>145</v>
       </c>
       <c r="B21" s="100">
@@ -39305,7 +39439,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="422" t="s">
+      <c r="A22" s="420" t="s">
         <v>146</v>
       </c>
       <c r="B22" s="100">
@@ -39330,7 +39464,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="424" t="s">
+      <c r="A23" s="422" t="s">
         <v>147</v>
       </c>
       <c r="B23" s="214">
@@ -39356,7 +39490,7 @@
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="429" t="s">
+      <c r="A27" s="427" t="s">
         <v>148</v>
       </c>
       <c r="B27" s="209">
@@ -39376,7 +39510,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="422" t="s">
+      <c r="A28" s="420" t="s">
         <v>149</v>
       </c>
       <c r="B28" s="100">
@@ -39401,7 +39535,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="422" t="s">
+      <c r="A29" s="420" t="s">
         <v>150</v>
       </c>
       <c r="B29" s="100">
@@ -39426,7 +39560,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="425" t="s">
+      <c r="A30" s="423" t="s">
         <v>151</v>
       </c>
       <c r="B30" s="216"/>
@@ -39448,7 +39582,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="426" t="s">
+      <c r="A31" s="424" t="s">
         <v>152</v>
       </c>
       <c r="B31" s="218"/>
@@ -39469,507 +39603,595 @@
         <v>1.1096668233542433</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="227" t="s">
+    <row r="32" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="564" t="s">
+        <v>330</v>
+      </c>
+      <c r="B32" s="565">
+        <f>(PASIVA!B3+PASIVA!B6)/'KAZALNIKI - PODJETJE X'!B29</f>
+        <v>1.5654143183581095</v>
+      </c>
+      <c r="C32" s="565">
+        <f>(PASIVA!C3+PASIVA!C6)/'KAZALNIKI - PODJETJE X'!C29</f>
+        <v>1.015625861530751</v>
+      </c>
+      <c r="D32" s="565">
+        <f>(PASIVA!D3+PASIVA!D6)/'KAZALNIKI - PODJETJE X'!D29</f>
+        <v>0.65281307357786678</v>
+      </c>
+      <c r="E32" s="565">
+        <f>(PASIVA!E3+PASIVA!E6)/'KAZALNIKI - PODJETJE X'!E29</f>
+        <v>1.0233419604197698</v>
+      </c>
+      <c r="F32" s="566">
+        <f>(PASIVA!F3+PASIVA!F6)/'KAZALNIKI - PODJETJE X'!F29</f>
+        <v>1.0543419990149776</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="461"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="227" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="209">
+      <c r="B35" s="209">
         <v>2013</v>
       </c>
-      <c r="C34" s="209">
+      <c r="C35" s="209">
         <v>2014</v>
       </c>
-      <c r="D34" s="209">
+      <c r="D35" s="209">
         <v>2015</v>
       </c>
-      <c r="E34" s="209">
+      <c r="E35" s="209">
         <v>2016</v>
       </c>
-      <c r="F34" s="210">
+      <c r="F35" s="210">
         <v>2017</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="430" t="s">
+    <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="428" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="220"/>
-      <c r="C35" s="220"/>
-      <c r="D35" s="220"/>
-      <c r="E35" s="220"/>
-      <c r="F35" s="221"/>
-    </row>
-    <row r="36" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="425" t="s">
+      <c r="B36" s="220"/>
+      <c r="C36" s="220"/>
+      <c r="D36" s="220"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="221"/>
+    </row>
+    <row r="37" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="423" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="216">
+      <c r="B37" s="216">
         <f>B21/B22</f>
         <v>1.5214517798186127</v>
       </c>
-      <c r="C36" s="216">
+      <c r="C37" s="216">
         <f>C21/C22</f>
         <v>1.5995777469078718</v>
       </c>
-      <c r="D36" s="216">
+      <c r="D37" s="216">
         <f>D21/D22</f>
         <v>1.5503669996803557</v>
       </c>
-      <c r="E36" s="216">
+      <c r="E37" s="216">
         <f>E21/E22</f>
         <v>1.3700387485177719</v>
       </c>
-      <c r="F36" s="217">
+      <c r="F37" s="217">
         <f>F21/F22</f>
         <v>1.261500923435332</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="427"/>
-      <c r="B37" s="137"/>
-      <c r="C37" s="137"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="137"/>
-      <c r="F37" s="222"/>
-    </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="430" t="s">
-        <v>156</v>
-      </c>
+      <c r="A38" s="425"/>
       <c r="B38" s="137"/>
       <c r="C38" s="137"/>
       <c r="D38" s="137"/>
       <c r="E38" s="137"/>
       <c r="F38" s="222"/>
     </row>
-    <row r="39" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="425" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="428" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="137"/>
+      <c r="C39" s="137"/>
+      <c r="D39" s="137"/>
+      <c r="E39" s="137"/>
+      <c r="F39" s="222"/>
+    </row>
+    <row r="40" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="423" t="s">
         <v>157</v>
       </c>
-      <c r="B39" s="216">
+      <c r="B40" s="216">
         <f>(B21-B11)/B22</f>
         <v>0.92093927984828095</v>
       </c>
-      <c r="C39" s="216">
+      <c r="C40" s="216">
         <f>(C21-C11)/C22</f>
         <v>0.96000790450061046</v>
       </c>
-      <c r="D39" s="216">
+      <c r="D40" s="216">
         <f>(D21-D11)/D22</f>
         <v>1.0241765790031805</v>
       </c>
-      <c r="E39" s="216">
+      <c r="E40" s="216">
         <f>(E21-E11)/E22</f>
         <v>0.82680750100789746</v>
       </c>
-      <c r="F39" s="217">
+      <c r="F40" s="217">
         <f>(F21-F11)/F22</f>
         <v>0.7613555611697832</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="427"/>
-      <c r="B40" s="137"/>
-      <c r="C40" s="137"/>
-      <c r="D40" s="137"/>
-      <c r="E40" s="137"/>
-      <c r="F40" s="222"/>
-    </row>
-    <row r="41" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="430" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="425"/>
+      <c r="B41" s="137"/>
+      <c r="C41" s="137"/>
+      <c r="D41" s="137"/>
+      <c r="E41" s="137"/>
+      <c r="F41" s="222"/>
+    </row>
+    <row r="42" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="428" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="220"/>
-      <c r="C41" s="220"/>
-      <c r="D41" s="220"/>
-      <c r="E41" s="220"/>
-      <c r="F41" s="221"/>
-    </row>
-    <row r="42" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="426" t="s">
+      <c r="B42" s="220"/>
+      <c r="C42" s="220"/>
+      <c r="D42" s="220"/>
+      <c r="E42" s="220"/>
+      <c r="F42" s="221"/>
+    </row>
+    <row r="43" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="424" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="218">
+      <c r="B43" s="218">
         <f>B15/B22</f>
         <v>9.4144900519652935E-2</v>
       </c>
-      <c r="C42" s="218">
+      <c r="C43" s="218">
         <f>C15/C22</f>
         <v>8.3581910409935734E-2</v>
       </c>
-      <c r="D42" s="218">
+      <c r="D43" s="218">
         <f>D15/D22</f>
         <v>0.13090219755202809</v>
       </c>
-      <c r="E42" s="218">
+      <c r="E43" s="218">
         <f>E15/E22</f>
         <v>0.10047632705706151</v>
       </c>
-      <c r="F42" s="219">
+      <c r="F43" s="219">
         <f>F15/F22</f>
         <v>7.9552739882009185E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="227" t="s">
+    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="227" t="s">
         <v>160</v>
       </c>
-      <c r="B47" s="209">
+      <c r="B48" s="209">
         <v>2013</v>
       </c>
-      <c r="C47" s="209">
+      <c r="C48" s="209">
         <v>2014</v>
       </c>
-      <c r="D47" s="209">
+      <c r="D48" s="209">
         <v>2015</v>
       </c>
-      <c r="E47" s="209">
+      <c r="E48" s="209">
         <v>2016</v>
       </c>
-      <c r="F47" s="210">
+      <c r="F48" s="210">
         <v>2017</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="430" t="s">
+    <row r="49" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="428" t="s">
         <v>161</v>
       </c>
-      <c r="B48" s="220"/>
-      <c r="C48" s="220"/>
-      <c r="D48" s="220"/>
-      <c r="E48" s="220"/>
-      <c r="F48" s="221"/>
-    </row>
-    <row r="49" spans="1:6" s="160" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="428" t="s">
+      <c r="B49" s="220"/>
+      <c r="C49" s="220"/>
+      <c r="D49" s="220"/>
+      <c r="E49" s="220"/>
+      <c r="F49" s="221"/>
+    </row>
+    <row r="50" spans="1:6" s="160" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="426" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="223">
+      <c r="B50" s="223">
         <f>(PASIVA!B5+PASIVA!B8)/AKTIVA!B17</f>
         <v>0.57886713264494705</v>
       </c>
-      <c r="C49" s="223">
+      <c r="C50" s="223">
         <f>(PASIVA!C5+PASIVA!C8)/AKTIVA!C17</f>
         <v>0.5115651321201512</v>
       </c>
-      <c r="D49" s="223">
+      <c r="D50" s="223">
         <f>(PASIVA!D5+PASIVA!D8)/AKTIVA!D17</f>
         <v>0.47652037155181509</v>
       </c>
-      <c r="E49" s="223">
+      <c r="E50" s="223">
         <f>(PASIVA!E5+PASIVA!E8)/AKTIVA!E17</f>
         <v>0.49957310180699172</v>
       </c>
-      <c r="F49" s="224">
+      <c r="F50" s="224">
         <f>(PASIVA!F5+PASIVA!F8)/AKTIVA!F17</f>
         <v>0.47849730663629536</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="227" t="s">
+    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="227" t="s">
         <v>163</v>
       </c>
-      <c r="B53" s="209">
+      <c r="B54" s="209">
         <v>2013</v>
       </c>
-      <c r="C53" s="209">
+      <c r="C54" s="209">
         <v>2014</v>
       </c>
-      <c r="D53" s="209">
+      <c r="D54" s="209">
         <v>2015</v>
       </c>
-      <c r="E53" s="209">
+      <c r="E54" s="209">
         <v>2016</v>
       </c>
-      <c r="F53" s="210">
+      <c r="F54" s="210">
         <v>2017</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="430" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="428" t="s">
         <v>164</v>
       </c>
-      <c r="B54" s="137"/>
-      <c r="C54" s="137"/>
-      <c r="D54" s="137"/>
-      <c r="E54" s="137"/>
-      <c r="F54" s="222"/>
-    </row>
-    <row r="55" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="425" t="s">
+      <c r="B55" s="137"/>
+      <c r="C55" s="137"/>
+      <c r="D55" s="137"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="222"/>
+    </row>
+    <row r="56" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="423" t="s">
         <v>165</v>
       </c>
-      <c r="B55" s="216">
-        <f>'FCF - KONČNI_IZRAČUN'!B5/'KAZALNIKI - PODJETJE X'!$B$61</f>
+      <c r="B56" s="216">
+        <f>'FCF - KONČNI_IZRAČUN'!B5/'KAZALNIKI - PODJETJE X'!$B$62</f>
         <v>3.7947073618181934E-2</v>
       </c>
-      <c r="C55" s="216">
-        <f>'FCF - KONČNI_IZRAČUN'!C5/'KAZALNIKI - PODJETJE X'!$B$61</f>
+      <c r="C56" s="216">
+        <f>'FCF - KONČNI_IZRAČUN'!C5/'KAZALNIKI - PODJETJE X'!$B$62</f>
         <v>8.2553842926136475E-2</v>
       </c>
-      <c r="D55" s="216">
-        <f>'FCF - KONČNI_IZRAČUN'!D5/'KAZALNIKI - PODJETJE X'!$B$61</f>
+      <c r="D56" s="216">
+        <f>'FCF - KONČNI_IZRAČUN'!D5/'KAZALNIKI - PODJETJE X'!$B$62</f>
         <v>0.11035562280454785</v>
       </c>
-      <c r="E55" s="216">
-        <f>'FCF - KONČNI_IZRAČUN'!E5/'KAZALNIKI - PODJETJE X'!$B$61</f>
+      <c r="E56" s="216">
+        <f>'FCF - KONČNI_IZRAČUN'!E5/'KAZALNIKI - PODJETJE X'!$B$62</f>
         <v>0.13438534630942367</v>
       </c>
-      <c r="F55" s="217">
-        <f>'FCF - KONČNI_IZRAČUN'!F5/'KAZALNIKI - PODJETJE X'!$B$61</f>
+      <c r="F56" s="217">
+        <f>'FCF - KONČNI_IZRAČUN'!F5/'KAZALNIKI - PODJETJE X'!$B$62</f>
         <v>0.14263410970579907</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="427"/>
-      <c r="B56" s="137"/>
-      <c r="C56" s="137"/>
-      <c r="D56" s="137"/>
-      <c r="E56" s="137"/>
-      <c r="F56" s="222"/>
-    </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="430" t="s">
-        <v>166</v>
-      </c>
+      <c r="A57" s="425"/>
       <c r="B57" s="137"/>
       <c r="C57" s="137"/>
       <c r="D57" s="137"/>
       <c r="E57" s="137"/>
       <c r="F57" s="222"/>
     </row>
-    <row r="58" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="426" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="428" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="137"/>
+      <c r="C58" s="137"/>
+      <c r="D58" s="137"/>
+      <c r="E58" s="137"/>
+      <c r="F58" s="222"/>
+    </row>
+    <row r="59" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="424" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="218">
-        <f>'FCF - KONČNI_IZRAČUN'!B5/'KAZALNIKI - PODJETJE X'!$B$64</f>
+      <c r="B59" s="218">
+        <f>'FCF - KONČNI_IZRAČUN'!B5/'KAZALNIKI - PODJETJE X'!$B$65</f>
         <v>7.6440562317114547E-2</v>
       </c>
-      <c r="C58" s="218">
-        <f>'FCF - KONČNI_IZRAČUN'!C5/'KAZALNIKI - PODJETJE X'!$B$64</f>
+      <c r="C59" s="218">
+        <f>'FCF - KONČNI_IZRAČUN'!C5/'KAZALNIKI - PODJETJE X'!$B$65</f>
         <v>0.16629641163394035</v>
       </c>
-      <c r="D58" s="218">
-        <f>'FCF - KONČNI_IZRAČUN'!D5/'KAZALNIKI - PODJETJE X'!$B$64</f>
+      <c r="D59" s="218">
+        <f>'FCF - KONČNI_IZRAČUN'!D5/'KAZALNIKI - PODJETJE X'!$B$65</f>
         <v>0.22230030033180678</v>
       </c>
-      <c r="E58" s="218">
-        <f>'FCF - KONČNI_IZRAČUN'!E5/'KAZALNIKI - PODJETJE X'!$B$64</f>
+      <c r="E59" s="218">
+        <f>'FCF - KONČNI_IZRAČUN'!E5/'KAZALNIKI - PODJETJE X'!$B$65</f>
         <v>0.27070576093516113</v>
       </c>
-      <c r="F58" s="219">
-        <f>'FCF - KONČNI_IZRAČUN'!F5/'KAZALNIKI - PODJETJE X'!$B$64</f>
+      <c r="F59" s="219">
+        <f>'FCF - KONČNI_IZRAČUN'!F5/'KAZALNIKI - PODJETJE X'!$B$65</f>
         <v>0.28732206496914736</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="161"/>
-      <c r="B60" s="162" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="161"/>
+      <c r="B61" s="162" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="163" t="s">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="163" t="s">
         <v>169</v>
       </c>
-      <c r="B61" s="164">
+      <c r="B62" s="164">
         <f>SUM(AKTIVA!B17:F17)/5</f>
         <v>76032002.599999994</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="161"/>
-      <c r="B63" s="162" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="161"/>
+      <c r="B64" s="162" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="163" t="s">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="163" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="164">
+      <c r="B65" s="164">
         <f>SUM(PASIVA!B25:F25)/5</f>
         <v>37744254</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="227" t="s">
+    <row r="68" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="227" t="s">
         <v>171</v>
       </c>
-      <c r="B68" s="209">
+      <c r="B69" s="209">
         <v>2013</v>
       </c>
-      <c r="C68" s="209">
+      <c r="C69" s="209">
         <v>2014</v>
       </c>
-      <c r="D68" s="209">
+      <c r="D69" s="209">
         <v>2015</v>
       </c>
-      <c r="E68" s="209">
+      <c r="E69" s="209">
         <v>2016</v>
       </c>
-      <c r="F68" s="210">
+      <c r="F69" s="210">
         <v>2017</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="430" t="s">
+    <row r="70" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="428" t="s">
         <v>239</v>
       </c>
-      <c r="B69" s="220"/>
-      <c r="C69" s="220"/>
-      <c r="D69" s="220"/>
-      <c r="E69" s="220"/>
-      <c r="F69" s="221"/>
-    </row>
-    <row r="70" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="425" t="s">
+      <c r="B70" s="220"/>
+      <c r="C70" s="220"/>
+      <c r="D70" s="220"/>
+      <c r="E70" s="220"/>
+      <c r="F70" s="221"/>
+    </row>
+    <row r="71" spans="1:6" s="159" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="423" t="s">
         <v>172</v>
       </c>
-      <c r="B70" s="216">
-        <f>'PRIHODKI IN STROŠKI'!B2/'KAZALNIKI - PODJETJE X'!$B$75</f>
+      <c r="B71" s="216">
+        <f>'PRIHODKI IN STROŠKI'!B2/'KAZALNIKI - PODJETJE X'!$B$76</f>
         <v>4.0307058360021433</v>
       </c>
-      <c r="C70" s="216">
-        <f>'PRIHODKI IN STROŠKI'!C2/'KAZALNIKI - PODJETJE X'!$B$75</f>
+      <c r="C71" s="216">
+        <f>'PRIHODKI IN STROŠKI'!C2/'KAZALNIKI - PODJETJE X'!$B$76</f>
         <v>4.4431984961209761</v>
       </c>
-      <c r="D70" s="216">
-        <f>'PRIHODKI IN STROŠKI'!D2/'KAZALNIKI - PODJETJE X'!$B$75</f>
+      <c r="D71" s="216">
+        <f>'PRIHODKI IN STROŠKI'!D2/'KAZALNIKI - PODJETJE X'!$B$76</f>
         <v>5.0973902888543376</v>
       </c>
-      <c r="E70" s="216">
-        <f>'PRIHODKI IN STROŠKI'!E2/'KAZALNIKI - PODJETJE X'!$B$75</f>
+      <c r="E71" s="216">
+        <f>'PRIHODKI IN STROŠKI'!E2/'KAZALNIKI - PODJETJE X'!$B$76</f>
         <v>5.8223343304106487</v>
       </c>
-      <c r="F70" s="217">
-        <f>'PRIHODKI IN STROŠKI'!F2/'KAZALNIKI - PODJETJE X'!$B$75</f>
+      <c r="F71" s="217">
+        <f>'PRIHODKI IN STROŠKI'!F2/'KAZALNIKI - PODJETJE X'!$B$76</f>
         <v>6.7058092670466412</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="426" t="s">
+    <row r="72" spans="1:6" s="159" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="424" t="s">
         <v>173</v>
       </c>
-      <c r="B71" s="218">
-        <f>365/B70</f>
+      <c r="B72" s="218">
+        <f>365/B71</f>
         <v>90.554859335015465</v>
       </c>
-      <c r="C71" s="218">
-        <f>365/C70</f>
+      <c r="C72" s="218">
+        <f>365/C71</f>
         <v>82.148029244845617</v>
       </c>
-      <c r="D71" s="218">
-        <f>365/D70</f>
+      <c r="D72" s="218">
+        <f>365/D71</f>
         <v>71.605268444538794</v>
       </c>
-      <c r="E71" s="218">
-        <f>365/E70</f>
+      <c r="E72" s="218">
+        <f>365/E71</f>
         <v>62.689632591788417</v>
       </c>
-      <c r="F71" s="219">
-        <f>365/F70</f>
+      <c r="F72" s="219">
+        <f>365/F71</f>
         <v>54.430417786211891</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F73" s="137"/>
-    </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="421"/>
-      <c r="B74" s="162" t="s">
+      <c r="F74" s="137"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="419"/>
+      <c r="B75" s="162" t="s">
         <v>168</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="220"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="163" t="s">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="220"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="163" t="s">
         <v>238</v>
       </c>
-      <c r="B75" s="164">
+      <c r="B76" s="164">
         <f>SUM(AKTIVA!B4:F4,AKTIVA!B9:F9)/5</f>
         <v>20781671.600000001</v>
       </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="100"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F76" s="137"/>
-    </row>
-    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="429" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="100"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F77" s="137"/>
+    </row>
+    <row r="78" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="427" t="s">
         <v>319</v>
       </c>
-      <c r="B78" s="209">
+      <c r="B79" s="209">
         <v>2013</v>
       </c>
-      <c r="C78" s="209">
+      <c r="C79" s="209">
         <v>2014</v>
       </c>
-      <c r="D78" s="209">
+      <c r="D79" s="209">
         <v>2015</v>
       </c>
-      <c r="E78" s="209">
+      <c r="E79" s="209">
         <v>2016</v>
       </c>
-      <c r="F78" s="210">
+      <c r="F79" s="210">
         <v>2017</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="427" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="425" t="s">
         <v>320</v>
       </c>
-      <c r="B79" s="137">
+      <c r="B80" s="137">
         <f>'FCF - KONČNI_IZRAČUN'!B5/'PRIHODKI IN STROŠKI'!B2</f>
         <v>3.4443964860898318E-2</v>
       </c>
-      <c r="C79" s="137">
+      <c r="C80" s="137">
         <f>'FCF - KONČNI_IZRAČUN'!C5/'PRIHODKI IN STROŠKI'!C2</f>
         <v>6.7976301441245307E-2</v>
       </c>
-      <c r="D79" s="137">
+      <c r="D80" s="137">
         <f>'FCF - KONČNI_IZRAČUN'!D5/'PRIHODKI IN STROŠKI'!D2</f>
         <v>7.9206811452798662E-2</v>
       </c>
-      <c r="E79" s="137">
+      <c r="E80" s="137">
         <f>'FCF - KONČNI_IZRAČUN'!E5/'PRIHODKI IN STROŠKI'!E2</f>
         <v>8.4444375205375566E-2</v>
       </c>
-      <c r="F79" s="222">
+      <c r="F80" s="222">
         <f>'FCF - KONČNI_IZRAČUN'!F5/'PRIHODKI IN STROŠKI'!F2</f>
         <v>7.7819448891626009E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="558"/>
-      <c r="B80" s="539"/>
-      <c r="C80" s="539"/>
-      <c r="D80" s="539"/>
-      <c r="E80" s="539"/>
-      <c r="F80" s="540"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81">
-        <f>AVERAGE(B79:F79)</f>
+    <row r="81" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="546"/>
+      <c r="B81" s="535"/>
+      <c r="C81" s="535"/>
+      <c r="D81" s="535"/>
+      <c r="E81" s="535"/>
+      <c r="F81" s="536"/>
+    </row>
+    <row r="82" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B82" s="545">
+        <f>AVERAGE(B80:F80)</f>
         <v>6.877818037038877E-2</v>
       </c>
     </row>
+    <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="559" t="s">
+        <v>322</v>
+      </c>
+      <c r="B88" s="560"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="B89" s="549">
+        <f>AVERAGE(AKTIVA!B17:F17)</f>
+        <v>76032002.599999994</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="B90" s="549">
+        <f>AVERAGE(PASIVA!B25:F25)</f>
+        <v>37744254</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="57"/>
+      <c r="B91" s="549"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="B92" s="549">
+        <f>'ANALIZA DELNICE'!G3*'ANALIZA DELNICE'!G9</f>
+        <v>2145767.7735000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="B93" s="549">
+        <f>AVERAGE('FCF - KONČNI_IZRAČUN'!B5:F5)</f>
+        <v>7722965.7999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="57" t="s">
+        <v>326</v>
+      </c>
+      <c r="B94" s="189">
+        <f>B82</f>
+        <v>6.877818037038877E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A88:B88"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -39978,7 +40200,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40030,23 +40252,23 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="434" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="470" t="s">
+    <row r="2" spans="1:12" s="432" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="468" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="466"/>
-      <c r="C2" s="466"/>
-      <c r="D2" s="466"/>
-      <c r="E2" s="466"/>
-      <c r="F2" s="471">
+      <c r="B2" s="464"/>
+      <c r="C2" s="464"/>
+      <c r="D2" s="464"/>
+      <c r="E2" s="464"/>
+      <c r="F2" s="469">
         <v>11421674</v>
       </c>
-      <c r="G2" s="467"/>
-      <c r="H2" s="466"/>
-      <c r="I2" s="466"/>
-      <c r="J2" s="466"/>
-      <c r="K2" s="468"/>
-      <c r="L2" s="469"/>
+      <c r="G2" s="465"/>
+      <c r="H2" s="464"/>
+      <c r="I2" s="464"/>
+      <c r="J2" s="464"/>
+      <c r="K2" s="466"/>
+      <c r="L2" s="467"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="50" t="s">
@@ -40554,7 +40776,7 @@
       <c r="F19" s="29"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="434"/>
+      <c r="G20" s="432"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40568,7 +40790,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40587,43 +40809,43 @@
       <c r="E2" t="s">
         <v>256</v>
       </c>
-      <c r="F2" s="444" t="s">
+      <c r="F2" s="442" t="s">
         <v>257</v>
       </c>
-      <c r="G2" s="489" t="s">
+      <c r="G2" s="487" t="s">
         <v>254</v>
       </c>
-      <c r="H2" s="489" t="s">
+      <c r="H2" s="487" t="s">
         <v>258</v>
       </c>
-      <c r="I2" s="489" t="s">
+      <c r="I2" s="487" t="s">
         <v>259</v>
       </c>
-      <c r="J2" s="490" t="s">
+      <c r="J2" s="488" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="434"/>
-      <c r="B3" s="444" t="s">
+      <c r="A3" s="432"/>
+      <c r="B3" s="442" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="482">
+      <c r="C3" s="480">
         <f>F5/H3</f>
         <v>1.8231347200545721E-2</v>
       </c>
       <c r="F3" s="57">
         <v>127169209</v>
       </c>
-      <c r="G3" s="464">
+      <c r="G3" s="462">
         <f>PASIVA!F25</f>
         <v>55347711</v>
       </c>
-      <c r="H3" s="464">
+      <c r="H3" s="462">
         <f>PASIVA!F3+PASIVA!F6</f>
         <v>19983877</v>
       </c>
-      <c r="I3" s="464">
+      <c r="I3" s="462">
         <f>'FCF - KONČNI_IZRAČUN'!F4</f>
         <v>703558</v>
       </c>
@@ -40633,31 +40855,31 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="434"/>
+      <c r="A4" s="432"/>
       <c r="B4" s="93" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="483">
+      <c r="C4" s="481">
         <f>I3/J3</f>
         <v>6.1598501235458132E-2</v>
       </c>
-      <c r="D4" s="492">
+      <c r="D4" s="490">
         <v>0.19</v>
       </c>
       <c r="F4" s="57" t="s">
         <v>260</v>
       </c>
-      <c r="G4" s="464"/>
-      <c r="H4" s="464"/>
-      <c r="I4" s="464"/>
+      <c r="G4" s="462"/>
+      <c r="H4" s="462"/>
+      <c r="I4" s="462"/>
       <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="434"/>
-      <c r="B5" s="472" t="s">
+      <c r="A5" s="432"/>
+      <c r="B5" s="470" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="484">
+      <c r="C5" s="482">
         <f>C3*(1-C4)</f>
         <v>1.710832353748884E-2</v>
       </c>
@@ -40665,55 +40887,55 @@
         <f>5603+358730</f>
         <v>364333</v>
       </c>
-      <c r="G5" s="465"/>
-      <c r="H5" s="465"/>
-      <c r="I5" s="465"/>
+      <c r="G5" s="463"/>
+      <c r="H5" s="463"/>
+      <c r="I5" s="463"/>
       <c r="J5" s="96"/>
     </row>
     <row r="6" spans="1:13" s="137" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="480"/>
-      <c r="B6" s="478"/>
-      <c r="C6" s="481"/>
+      <c r="A6" s="478"/>
+      <c r="B6" s="476"/>
+      <c r="C6" s="479"/>
     </row>
     <row r="7" spans="1:13" s="137" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="480"/>
-      <c r="B7" s="478"/>
-      <c r="C7" s="481"/>
+      <c r="A7" s="478"/>
+      <c r="B7" s="476"/>
+      <c r="C7" s="479"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="444" t="s">
+      <c r="B8" s="442" t="s">
         <v>245</v>
       </c>
-      <c r="C8" s="502">
+      <c r="C8" s="500">
         <f>F9</f>
         <v>1.01</v>
       </c>
-      <c r="F8" s="444" t="s">
+      <c r="F8" s="442" t="s">
         <v>245</v>
       </c>
-      <c r="G8" s="489" t="s">
+      <c r="G8" s="487" t="s">
         <v>267</v>
       </c>
-      <c r="H8" s="490" t="s">
+      <c r="H8" s="488" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="473" t="s">
+      <c r="B9" s="471" t="s">
         <v>269</v>
       </c>
-      <c r="C9" s="503">
+      <c r="C9" s="501">
         <f>H9</f>
         <v>1.3522079935556053</v>
       </c>
-      <c r="F9" s="491">
+      <c r="F9" s="489">
         <v>1.01</v>
       </c>
       <c r="G9" s="175">
         <f>C11/C10</f>
         <v>0.36106058658866663</v>
       </c>
-      <c r="H9" s="522">
+      <c r="H9" s="518">
         <f>C8*(1+(1-C4)*G9)</f>
         <v>1.3522079935556053</v>
       </c>
@@ -40722,7 +40944,7 @@
       <c r="B10" s="57" t="s">
         <v>263</v>
       </c>
-      <c r="C10" s="485">
+      <c r="C10" s="483">
         <f>G3/(G3+H3)</f>
         <v>0.73472115044222885</v>
       </c>
@@ -40731,7 +40953,7 @@
       <c r="B11" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="C11" s="486">
+      <c r="C11" s="484">
         <f>H3/(H3+G3)</f>
         <v>0.26527884955777115</v>
       </c>
@@ -40740,51 +40962,51 @@
       <c r="B12" s="57" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="520">
+      <c r="C12" s="516">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="F12" s="544" t="s">
+      <c r="F12" s="551" t="s">
         <v>272</v>
       </c>
-      <c r="G12" s="545"/>
-      <c r="H12" s="546"/>
-      <c r="J12" s="512" t="s">
+      <c r="G12" s="552"/>
+      <c r="H12" s="553"/>
+      <c r="J12" s="508" t="s">
         <v>286</v>
       </c>
-      <c r="K12" s="514"/>
-      <c r="L12" s="514"/>
-      <c r="M12" s="507"/>
+      <c r="K12" s="510"/>
+      <c r="L12" s="510"/>
+      <c r="M12" s="505"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="C13" s="520">
+      <c r="C13" s="516">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="F13" s="496">
+      <c r="F13" s="494">
         <v>42736</v>
       </c>
-      <c r="G13" s="497">
+      <c r="G13" s="495">
         <v>8.6E-3</v>
       </c>
-      <c r="H13" s="501">
+      <c r="H13" s="499">
         <f>AVERAGE(G13:G24)</f>
         <v>9.9416666666666664E-3</v>
       </c>
-      <c r="J13" s="513">
+      <c r="J13" s="509">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="475" t="s">
+      <c r="B14" s="473" t="s">
         <v>248</v>
       </c>
-      <c r="C14" s="504">
+      <c r="C14" s="502">
         <f>J13</f>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F14" s="494">
+      <c r="F14" s="492">
         <v>42767</v>
       </c>
       <c r="G14" s="173">
@@ -40792,50 +41014,50 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="475" t="s">
+      <c r="B15" s="473" t="s">
         <v>249</v>
       </c>
-      <c r="C15" s="504">
+      <c r="C15" s="502">
         <f>J16</f>
         <v>0.05</v>
       </c>
-      <c r="F15" s="494">
+      <c r="F15" s="492">
         <v>42795</v>
       </c>
       <c r="G15" s="173">
         <v>1.03E-2</v>
       </c>
-      <c r="J15" s="544" t="s">
+      <c r="J15" s="551" t="s">
         <v>293</v>
       </c>
-      <c r="K15" s="545"/>
-      <c r="L15" s="545"/>
-      <c r="M15" s="546"/>
+      <c r="K15" s="552"/>
+      <c r="L15" s="552"/>
+      <c r="M15" s="553"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="476" t="s">
+      <c r="B16" s="474" t="s">
         <v>250</v>
       </c>
-      <c r="C16" s="521"/>
-      <c r="F16" s="494">
+      <c r="C16" s="517"/>
+      <c r="F16" s="492">
         <v>42826</v>
       </c>
       <c r="G16" s="173">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="J16" s="513">
+      <c r="J16" s="509">
         <v>0.05</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="477" t="s">
+      <c r="B17" s="475" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="487">
+      <c r="C17" s="485">
         <f>C12+C13+C14+C15*C9</f>
         <v>0.15501039967778027</v>
       </c>
-      <c r="F17" s="494">
+      <c r="F17" s="492">
         <v>42856</v>
       </c>
       <c r="G17" s="173">
@@ -40843,9 +41065,9 @@
       </c>
     </row>
     <row r="18" spans="2:9" s="137" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="478"/>
-      <c r="C18" s="479"/>
-      <c r="F18" s="494">
+      <c r="B18" s="476"/>
+      <c r="C18" s="477"/>
+      <c r="F18" s="492">
         <v>42887</v>
       </c>
       <c r="G18" s="173">
@@ -40853,230 +41075,230 @@
       </c>
     </row>
     <row r="19" spans="2:9" s="137" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="478"/>
-      <c r="C19" s="479"/>
-      <c r="F19" s="494">
+      <c r="B19" s="476"/>
+      <c r="C19" s="477"/>
+      <c r="F19" s="492">
         <v>42917</v>
       </c>
-      <c r="G19" s="498">
+      <c r="G19" s="496">
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="488" t="s">
+      <c r="B20" s="486" t="s">
         <v>251</v>
       </c>
-      <c r="C20" s="487">
+      <c r="C20" s="485">
         <f>C17*C10+C5*C11*(1-D4)</f>
         <v>0.11756558505433704</v>
       </c>
-      <c r="F20" s="494">
+      <c r="F20" s="492">
         <v>42948</v>
       </c>
-      <c r="G20" s="498">
+      <c r="G20" s="496">
         <v>1.12E-2</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F21" s="494">
+      <c r="F21" s="492">
         <v>42979</v>
       </c>
-      <c r="G21" s="498">
+      <c r="G21" s="496">
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F22" s="494">
+      <c r="F22" s="492">
         <v>43009</v>
       </c>
-      <c r="G22" s="499">
+      <c r="G22" s="497">
         <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F23" s="494">
+      <c r="F23" s="492">
         <v>43040</v>
       </c>
-      <c r="G23" s="498">
+      <c r="G23" s="496">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="495">
+      <c r="F24" s="493">
         <v>43070</v>
       </c>
-      <c r="G24" s="500">
+      <c r="G24" s="498">
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="515"/>
-      <c r="G25" s="516"/>
+      <c r="F25" s="511"/>
+      <c r="G25" s="512"/>
     </row>
     <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="547" t="s">
+      <c r="F26" s="554" t="s">
         <v>285</v>
       </c>
-      <c r="G26" s="548"/>
-      <c r="H26" s="549"/>
+      <c r="G26" s="555"/>
+      <c r="H26" s="556"/>
     </row>
     <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F27" s="517">
+      <c r="F27" s="513">
         <v>42737</v>
       </c>
-      <c r="G27" s="518">
+      <c r="G27" s="514">
         <v>5.6899999999999999E-2</v>
       </c>
-      <c r="H27" s="511">
+      <c r="H27" s="507">
         <f>AVERAGE(G27:G38)</f>
         <v>5.1233333333333332E-2</v>
       </c>
-      <c r="I27" s="510"/>
+      <c r="I27" s="506"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F28" s="494">
+      <c r="F28" s="492">
         <v>42769</v>
       </c>
-      <c r="G28" s="498">
+      <c r="G28" s="496">
         <v>5.5899999999999998E-2</v>
       </c>
-      <c r="I28" s="510"/>
+      <c r="I28" s="506"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F29" s="494">
+      <c r="F29" s="492">
         <v>42795</v>
       </c>
-      <c r="G29" s="498">
+      <c r="G29" s="496">
         <v>5.3900000000000003E-2</v>
       </c>
-      <c r="I29" s="510"/>
+      <c r="I29" s="506"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F30" s="494">
+      <c r="F30" s="492">
         <v>42826</v>
       </c>
-      <c r="G30" s="498">
+      <c r="G30" s="496">
         <v>5.3800000000000001E-2</v>
       </c>
-      <c r="I30" s="510"/>
+      <c r="I30" s="506"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F31" s="494">
+      <c r="F31" s="492">
         <v>42856</v>
       </c>
-      <c r="G31" s="498">
+      <c r="G31" s="496">
         <v>4.87E-2</v>
       </c>
-      <c r="I31" s="510"/>
+      <c r="I31" s="506"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F32" s="494">
+      <c r="F32" s="492">
         <v>42888</v>
       </c>
-      <c r="G32" s="498">
+      <c r="G32" s="496">
         <v>5.2900000000000003E-2</v>
       </c>
-      <c r="I32" s="510"/>
+      <c r="I32" s="506"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F33" s="494">
+      <c r="F33" s="492">
         <v>42919</v>
       </c>
-      <c r="G33" s="498">
+      <c r="G33" s="496">
         <v>5.1299999999999998E-2</v>
       </c>
-      <c r="I33" s="510"/>
+      <c r="I33" s="506"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F34" s="494">
+      <c r="F34" s="492">
         <v>42948</v>
       </c>
-      <c r="G34" s="498">
+      <c r="G34" s="496">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="I34" s="510"/>
+      <c r="I34" s="506"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F35" s="494">
+      <c r="F35" s="492">
         <v>42982</v>
       </c>
-      <c r="G35" s="498">
+      <c r="G35" s="496">
         <v>5.04E-2</v>
       </c>
-      <c r="I35" s="510"/>
+      <c r="I35" s="506"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F36" s="494">
+      <c r="F36" s="492">
         <v>43012</v>
       </c>
-      <c r="G36" s="498">
+      <c r="G36" s="496">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="I36" s="510"/>
+      <c r="I36" s="506"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F37" s="494">
+      <c r="F37" s="492">
         <v>43040</v>
       </c>
-      <c r="G37" s="498">
+      <c r="G37" s="496">
         <v>4.8099999999999997E-2</v>
       </c>
-      <c r="I37" s="510"/>
+      <c r="I37" s="506"/>
     </row>
     <row r="38" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F38" s="495">
+      <c r="F38" s="493">
         <v>43070</v>
       </c>
-      <c r="G38" s="500">
+      <c r="G38" s="498">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="I38" s="519"/>
+      <c r="I38" s="515"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F39" s="515"/>
-      <c r="G39" s="516"/>
+      <c r="F39" s="511"/>
+      <c r="G39" s="512"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F40" s="515"/>
-      <c r="G40" s="516"/>
+      <c r="F40" s="511"/>
+      <c r="G40" s="512"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F41" s="515"/>
-      <c r="G41" s="516"/>
+      <c r="F41" s="511"/>
+      <c r="G41" s="512"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F42" s="515"/>
-      <c r="G42" s="516"/>
+      <c r="F42" s="511"/>
+      <c r="G42" s="512"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>270</v>
       </c>
-      <c r="F43" s="515"/>
-      <c r="G43" s="516"/>
+      <c r="F43" s="511"/>
+      <c r="G43" s="512"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="493" t="s">
+      <c r="B44" s="491" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="493" t="s">
+      <c r="B45" s="491" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="493" t="s">
+      <c r="B46" s="491" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="493" t="s">
+      <c r="B47" s="491" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="493" t="s">
+      <c r="B48" s="491" t="s">
         <v>294</v>
       </c>
     </row>
@@ -41104,7 +41326,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41115,7 +41337,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="535" t="s">
+      <c r="B1" s="531" t="s">
         <v>295</v>
       </c>
     </row>
@@ -41125,25 +41347,25 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="493" t="s">
+      <c r="B3" s="491" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="532"/>
-      <c r="B7" s="533" t="s">
+      <c r="A7" s="528"/>
+      <c r="B7" s="529" t="s">
         <v>298</v>
       </c>
-      <c r="C7" s="534" t="s">
+      <c r="C7" s="530" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="550" t="s">
+      <c r="A8" s="557" t="s">
         <v>308</v>
       </c>
-      <c r="B8" s="464" t="s">
+      <c r="B8" s="462" t="s">
         <v>300</v>
       </c>
       <c r="C8" s="56" t="s">
@@ -41151,8 +41373,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="550"/>
-      <c r="B9" s="464" t="s">
+      <c r="A9" s="557"/>
+      <c r="B9" s="462" t="s">
         <v>304</v>
       </c>
       <c r="C9" s="56" t="s">
@@ -41160,8 +41382,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="550"/>
-      <c r="B10" s="464" t="s">
+      <c r="A10" s="557"/>
+      <c r="B10" s="462" t="s">
         <v>305</v>
       </c>
       <c r="C10" s="56" t="s">
@@ -41169,102 +41391,102 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="551"/>
-      <c r="B11" s="465" t="s">
+      <c r="A11" s="558"/>
+      <c r="B11" s="463" t="s">
         <v>306</v>
       </c>
       <c r="C11" s="96"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="541"/>
-      <c r="B13" s="542" t="s">
+      <c r="A13" s="537"/>
+      <c r="B13" s="538" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="543"/>
+      <c r="C13" s="539"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="536" t="s">
+      <c r="A14" s="532" t="s">
         <v>310</v>
       </c>
-      <c r="B14" s="537" t="s">
+      <c r="B14" s="533" t="s">
         <v>307</v>
       </c>
       <c r="C14" s="222"/>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="538" t="s">
+      <c r="A15" s="534" t="s">
         <v>311</v>
       </c>
-      <c r="B15" s="552" t="s">
+      <c r="B15" s="540" t="s">
         <v>312</v>
       </c>
       <c r="C15" s="222"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="536"/>
-      <c r="B16" s="552" t="s">
+      <c r="A16" s="532"/>
+      <c r="B16" s="540" t="s">
         <v>313</v>
       </c>
       <c r="C16" s="222"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="536"/>
-      <c r="B17" s="552" t="s">
+      <c r="A17" s="532"/>
+      <c r="B17" s="540" t="s">
         <v>314</v>
       </c>
       <c r="C17" s="222"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="536"/>
-      <c r="B18" s="552" t="s">
+      <c r="A18" s="532"/>
+      <c r="B18" s="540" t="s">
         <v>315</v>
       </c>
       <c r="C18" s="222"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="536"/>
-      <c r="B19" s="552" t="s">
+      <c r="A19" s="532"/>
+      <c r="B19" s="540" t="s">
         <v>316</v>
       </c>
       <c r="C19" s="222"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="536"/>
-      <c r="B20" s="552" t="s">
+      <c r="A20" s="532"/>
+      <c r="B20" s="540" t="s">
         <v>317</v>
       </c>
       <c r="C20" s="222"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="536"/>
-      <c r="B21" s="552"/>
+      <c r="A21" s="532"/>
+      <c r="B21" s="540"/>
       <c r="C21" s="222"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="536"/>
-      <c r="B22" s="552"/>
+      <c r="A22" s="532"/>
+      <c r="B22" s="540"/>
       <c r="C22" s="222"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="536"/>
-      <c r="B23" s="552"/>
+      <c r="A23" s="532"/>
+      <c r="B23" s="540"/>
       <c r="C23" s="222"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="536"/>
-      <c r="B24" s="552"/>
+      <c r="A24" s="532"/>
+      <c r="B24" s="540"/>
       <c r="C24" s="222"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="536"/>
-      <c r="B25" s="552"/>
+      <c r="A25" s="532"/>
+      <c r="B25" s="540"/>
       <c r="C25" s="222"/>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="538"/>
-      <c r="B26" s="553"/>
-      <c r="C26" s="540"/>
+      <c r="A26" s="534"/>
+      <c r="B26" s="541"/>
+      <c r="C26" s="536"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -41295,52 +41517,53 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26207D2D-D345-4415-BB7E-16436BF85CD2}">
-  <dimension ref="B1:G17"/>
+  <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="46.44140625" customWidth="1"/>
+    <col min="3" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="505">
+      <c r="C2" s="503">
         <v>2013</v>
       </c>
-      <c r="D2" s="506">
+      <c r="D2" s="504">
         <v>2014</v>
       </c>
-      <c r="E2" s="506">
+      <c r="E2" s="504">
         <v>2015</v>
       </c>
-      <c r="F2" s="506">
+      <c r="F2" s="504">
         <v>2016</v>
       </c>
-      <c r="G2" s="507">
+      <c r="G2" s="505">
         <v>2017</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="444" t="s">
+      <c r="B3" s="442" t="s">
         <v>281</v>
       </c>
-      <c r="C3" s="489">
+      <c r="C3" s="487">
         <v>514215</v>
       </c>
-      <c r="D3" s="489">
+      <c r="D3" s="487">
         <v>514215</v>
       </c>
-      <c r="E3" s="489">
+      <c r="E3" s="487">
         <v>514215</v>
       </c>
-      <c r="F3" s="489">
+      <c r="F3" s="487">
         <v>514215</v>
       </c>
-      <c r="G3" s="490">
+      <c r="G3" s="488">
         <v>514215</v>
       </c>
     </row>
@@ -41348,16 +41571,16 @@
       <c r="B4" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="C4" s="464">
+      <c r="C4" s="462">
         <v>38105</v>
       </c>
-      <c r="D4" s="464">
+      <c r="D4" s="462">
         <v>8911</v>
       </c>
-      <c r="E4" s="464">
+      <c r="E4" s="462">
         <v>157</v>
       </c>
-      <c r="F4" s="464">
+      <c r="F4" s="462">
         <v>580</v>
       </c>
       <c r="G4" s="56">
@@ -41368,16 +41591,16 @@
       <c r="B5" s="57" t="s">
         <v>282</v>
       </c>
-      <c r="C5" s="464">
+      <c r="C5" s="462">
         <v>209567</v>
       </c>
-      <c r="D5" s="464">
+      <c r="D5" s="462">
         <v>49000</v>
       </c>
-      <c r="E5" s="464">
+      <c r="E5" s="462">
         <v>1372</v>
       </c>
-      <c r="F5" s="464">
+      <c r="F5" s="462">
         <v>3699</v>
       </c>
       <c r="G5" s="56">
@@ -41385,205 +41608,255 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="440" t="s">
+      <c r="B6" s="438" t="s">
         <v>292</v>
       </c>
-      <c r="C6" s="530">
+      <c r="C6" s="526">
         <v>64471</v>
       </c>
-      <c r="D6" s="530">
+      <c r="D6" s="526">
         <v>-37933</v>
       </c>
-      <c r="E6" s="530">
+      <c r="E6" s="526">
         <v>63700</v>
       </c>
-      <c r="F6" s="530">
+      <c r="F6" s="526">
         <v>935</v>
       </c>
-      <c r="G6" s="531">
+      <c r="G6" s="527">
         <v>29160</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="440" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="C7" s="508">
+      <c r="C7" s="170">
         <v>9.7699999999999995E-2</v>
       </c>
-      <c r="D7" s="508">
+      <c r="D7" s="170">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="E7" s="508">
+      <c r="E7" s="170">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F7" s="508">
+      <c r="F7" s="170">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="G7" s="509">
+      <c r="G7" s="472">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="444" t="s">
+    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="474" t="s">
+        <v>321</v>
+      </c>
+      <c r="C8" s="547">
+        <f>1-C4/C3</f>
+        <v>0.92589675524829107</v>
+      </c>
+      <c r="D8" s="547">
+        <f t="shared" ref="D8:G8" si="0">1-D4/D3</f>
+        <v>0.98267067277306186</v>
+      </c>
+      <c r="E8" s="547">
+        <f t="shared" si="0"/>
+        <v>0.99969468024075536</v>
+      </c>
+      <c r="F8" s="547">
+        <f t="shared" si="0"/>
+        <v>0.99887206713145282</v>
+      </c>
+      <c r="G8" s="548">
+        <f t="shared" si="0"/>
+        <v>0.99872815845512086</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="442" t="s">
         <v>275</v>
       </c>
-      <c r="C8" s="489">
+      <c r="C9" s="487">
         <v>4.1729000000000003</v>
       </c>
-      <c r="D8" s="489">
+      <c r="D9" s="487">
         <v>4.1729000000000003</v>
       </c>
-      <c r="E8" s="489">
+      <c r="E9" s="487">
         <v>4.1729000000000003</v>
       </c>
-      <c r="F8" s="489">
+      <c r="F9" s="487">
         <v>4.1729000000000003</v>
       </c>
-      <c r="G8" s="490">
+      <c r="G9" s="488">
         <v>4.1729000000000003</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="57" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="C9" s="464">
+      <c r="C10" s="462">
         <v>5.5</v>
       </c>
-      <c r="D9" s="464">
+      <c r="D10" s="462">
         <v>5.5</v>
       </c>
-      <c r="E9" s="464" t="s">
+      <c r="E10" s="462" t="s">
         <v>279</v>
       </c>
-      <c r="F9" s="464" t="s">
+      <c r="F10" s="462" t="s">
         <v>279</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G10" s="56" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="93" t="s">
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="93" t="s">
         <v>278</v>
       </c>
-      <c r="C10" s="465" t="s">
+      <c r="C11" s="463" t="s">
         <v>280</v>
       </c>
-      <c r="D10" s="465" t="s">
+      <c r="D11" s="463" t="s">
         <v>280</v>
       </c>
-      <c r="E10" s="465">
+      <c r="E11" s="463">
         <v>5.5</v>
       </c>
-      <c r="F10" s="465" t="s">
+      <c r="F11" s="463" t="s">
         <v>280</v>
       </c>
-      <c r="G10" s="96" t="s">
+      <c r="G11" s="96" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="283" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="550">
+        <f>C3*C9-C5</f>
+        <v>1936200.7735000001</v>
+      </c>
+      <c r="D12" s="550">
+        <f t="shared" ref="D12:G12" si="1">D3*D9-D5</f>
+        <v>2096767.7735000001</v>
+      </c>
+      <c r="E12" s="550">
+        <f t="shared" si="1"/>
+        <v>2144395.7735000001</v>
+      </c>
+      <c r="F12" s="550">
+        <f t="shared" si="1"/>
+        <v>2142068.7735000001</v>
+      </c>
+      <c r="G12" s="550">
+        <f t="shared" si="1"/>
+        <v>2143782.7735000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="283" t="s">
         <v>287</v>
       </c>
-      <c r="C13" s="523">
+      <c r="C14" s="519">
         <v>2013</v>
       </c>
-      <c r="D13" s="524">
+      <c r="D14" s="520">
         <v>2014</v>
       </c>
-      <c r="E13" s="524">
+      <c r="E14" s="520">
         <v>2015</v>
       </c>
-      <c r="F13" s="524">
+      <c r="F14" s="520">
         <v>2016</v>
       </c>
-      <c r="G13" s="525">
+      <c r="G14" s="521">
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="444" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="442" t="s">
         <v>288</v>
       </c>
-      <c r="C14" s="527">
+      <c r="C15" s="523">
         <v>0.59040000000000004</v>
       </c>
-      <c r="D14" s="527">
+      <c r="D15" s="523">
         <v>0.62560000000000004</v>
       </c>
-      <c r="E14" s="527">
+      <c r="E15" s="523">
         <v>0.62560000000000004</v>
       </c>
-      <c r="F14" s="527">
+      <c r="F15" s="523">
         <v>0.5877</v>
       </c>
-      <c r="G14" s="528">
+      <c r="G15" s="524">
         <v>0.52659999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="57" t="s">
-        <v>289</v>
-      </c>
-      <c r="C15" s="170">
-        <v>0.1968</v>
-      </c>
-      <c r="D15" s="170">
-        <v>0.2198</v>
-      </c>
-      <c r="E15" s="170">
-        <v>0.2198</v>
-      </c>
-      <c r="F15" s="170">
-        <v>0.26040000000000002</v>
-      </c>
-      <c r="G15" s="474">
-        <v>0.30509999999999998</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="170">
+        <v>0.1968</v>
+      </c>
+      <c r="D16" s="170">
+        <v>0.2198</v>
+      </c>
+      <c r="E16" s="170">
+        <v>0.2198</v>
+      </c>
+      <c r="F16" s="170">
+        <v>0.26040000000000002</v>
+      </c>
+      <c r="G16" s="472">
+        <v>0.30509999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="57" t="s">
         <v>290</v>
       </c>
-      <c r="C16" s="526">
+      <c r="C17" s="522">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="D16" s="170">
+      <c r="D17" s="170">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="E16" s="170">
+      <c r="E17" s="170">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="F16" s="526">
+      <c r="F17" s="522">
         <v>7.5700000000000003E-2</v>
       </c>
-      <c r="G16" s="474">
+      <c r="G17" s="472">
         <v>9.06E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="93" t="s">
+    <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="93" t="s">
         <v>291</v>
       </c>
-      <c r="C17" s="175">
+      <c r="C18" s="175">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="D17" s="175">
+      <c r="D18" s="175">
         <v>7.0599999999999996E-2</v>
       </c>
-      <c r="E17" s="175">
+      <c r="E18" s="175">
         <v>7.0599999999999996E-2</v>
       </c>
-      <c r="F17" s="175">
+      <c r="F18" s="175">
         <v>7.51E-2</v>
       </c>
-      <c r="G17" s="529">
+      <c r="G18" s="525">
         <v>7.6399999999999996E-2</v>
       </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="506"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
@@ -41597,7 +41870,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41723,7 +41996,7 @@
       <c r="K3" s="34">
         <v>1.1200000000000001</v>
       </c>
-      <c r="L3" s="434"/>
+      <c r="L3" s="432"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="356" t="s">
@@ -41893,6 +42166,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="461"/>
       <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -42342,11 +42616,11 @@
         <v>203</v>
       </c>
       <c r="B23" s="41">
-        <f t="shared" ref="B23:K23" si="9">SUM(B19:B22)+B12</f>
+        <f>SUM(B19:B22)+B12</f>
         <v>84260931</v>
       </c>
       <c r="C23" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="B23:K23" si="9">SUM(C19:C22)+C12</f>
         <v>90935185</v>
       </c>
       <c r="D23" s="41">
@@ -42608,7 +42882,7 @@
       <c r="K31" s="248">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L31" s="434"/>
+      <c r="L31" s="432"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="174" t="s">
@@ -42840,7 +43114,7 @@
         <v>207</v>
       </c>
       <c r="B38" s="349">
-        <f t="shared" si="19"/>
+        <f>B23/B$6</f>
         <v>0.96991077863314534</v>
       </c>
       <c r="C38" s="349">
@@ -42948,10 +43222,10 @@
       <c r="E42" s="8">
         <v>30776943</v>
       </c>
-      <c r="F42" s="447">
+      <c r="F42" s="445">
         <v>34236712</v>
       </c>
-      <c r="G42" s="452">
+      <c r="G42" s="450">
         <f>G43*G44</f>
         <v>37202109.690460496</v>
       </c>
@@ -42971,7 +43245,7 @@
         <f>K43*K44</f>
         <v>51864434.442043714</v>
       </c>
-      <c r="L42" s="451">
+      <c r="L42" s="449">
         <f>SUM(C46:F46)/4</f>
         <v>1.0549655906657875</v>
       </c>
@@ -42992,10 +43266,10 @@
       <c r="E43" s="204">
         <v>1225</v>
       </c>
-      <c r="F43" s="448">
+      <c r="F43" s="446">
         <v>1265</v>
       </c>
-      <c r="G43" s="453">
+      <c r="G43" s="451">
         <f>G45*F43</f>
         <v>1302.95</v>
       </c>
@@ -43040,7 +43314,7 @@
         <f>F42/F43</f>
         <v>27064.594466403163</v>
       </c>
-      <c r="G44" s="454">
+      <c r="G44" s="452">
         <f>F44*G46</f>
         <v>28552.215887379018</v>
       </c>
@@ -43078,109 +43352,109 @@
         <f>E43/D43</f>
         <v>1.1279926335174955</v>
       </c>
-      <c r="F45" s="449">
+      <c r="F45" s="447">
         <f>F43/E43</f>
         <v>1.0326530612244897</v>
       </c>
-      <c r="G45" s="455">
+      <c r="G45" s="453">
         <v>1.03</v>
       </c>
-      <c r="H45" s="455">
+      <c r="H45" s="453">
         <v>1.03</v>
       </c>
-      <c r="I45" s="455">
+      <c r="I45" s="453">
         <v>1.03</v>
       </c>
-      <c r="J45" s="455">
+      <c r="J45" s="453">
         <v>1.03</v>
       </c>
-      <c r="K45" s="455">
+      <c r="K45" s="453">
         <v>1.03</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="440" t="s">
+      <c r="A46" s="438" t="s">
         <v>231</v>
       </c>
-      <c r="B46" s="441"/>
-      <c r="C46" s="442">
+      <c r="B46" s="439"/>
+      <c r="C46" s="440">
         <f>C44/B44</f>
         <v>1.0342314877652128</v>
       </c>
-      <c r="D46" s="442">
+      <c r="D46" s="440">
         <f t="shared" ref="D46:F46" si="23">D44/C44</f>
         <v>1.0623203617402275</v>
       </c>
-      <c r="E46" s="442">
+      <c r="E46" s="440">
         <f t="shared" si="23"/>
         <v>1.0460713532663635</v>
       </c>
-      <c r="F46" s="450">
+      <c r="F46" s="448">
         <f t="shared" si="23"/>
         <v>1.0772391598913471</v>
       </c>
-      <c r="G46" s="456">
+      <c r="G46" s="454">
         <f>$L$42</f>
         <v>1.0549655906657875</v>
       </c>
-      <c r="H46" s="443">
+      <c r="H46" s="441">
         <f t="shared" ref="H46:K46" si="24">$L$42</f>
         <v>1.0549655906657875</v>
       </c>
-      <c r="I46" s="443">
+      <c r="I46" s="441">
         <f t="shared" si="24"/>
         <v>1.0549655906657875</v>
       </c>
-      <c r="J46" s="443">
+      <c r="J46" s="441">
         <f t="shared" si="24"/>
         <v>1.0549655906657875</v>
       </c>
-      <c r="K46" s="457">
+      <c r="K46" s="455">
         <f t="shared" si="24"/>
         <v>1.0549655906657875</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="444" t="s">
+      <c r="A47" s="442" t="s">
         <v>242</v>
       </c>
-      <c r="B47" s="445">
+      <c r="B47" s="443">
         <f>B2/B43</f>
         <v>82608.288954635107</v>
       </c>
-      <c r="C47" s="445">
+      <c r="C47" s="443">
         <f t="shared" ref="C47:K47" si="25">C2/C43</f>
         <v>86457.951310861419</v>
       </c>
-      <c r="D47" s="445">
+      <c r="D47" s="443">
         <f t="shared" si="25"/>
         <v>97543.546040515648</v>
       </c>
-      <c r="E47" s="445">
+      <c r="E47" s="443">
         <f t="shared" si="25"/>
         <v>98773.746938775512</v>
       </c>
-      <c r="F47" s="446">
+      <c r="F47" s="444">
         <f t="shared" si="25"/>
         <v>110164.36837944663</v>
       </c>
-      <c r="G47" s="458">
+      <c r="G47" s="456">
         <f t="shared" si="25"/>
         <v>120859.93812502398</v>
       </c>
-      <c r="H47" s="445">
+      <c r="H47" s="443">
         <f t="shared" si="25"/>
         <v>131420.51524274453</v>
       </c>
-      <c r="I47" s="445">
+      <c r="I47" s="443">
         <f t="shared" si="25"/>
         <v>142903.861234829</v>
       </c>
-      <c r="J47" s="445">
+      <c r="J47" s="443">
         <f t="shared" si="25"/>
         <v>155390.60639127038</v>
       </c>
-      <c r="K47" s="446">
+      <c r="K47" s="444">
         <f t="shared" si="25"/>
         <v>168968.42636720664</v>
       </c>
@@ -43209,7 +43483,7 @@
         <f>'FCF - KONČNI_IZRAČUN'!F5/'PRIHODKI IN STROŠKI'!F43</f>
         <v>8572.9304347826092</v>
       </c>
-      <c r="G48" s="459">
+      <c r="G48" s="457">
         <f>'FCF - KONČNI_IZRAČUN'!G5/'PRIHODKI IN STROŠKI'!G43</f>
         <v>10190.756758657404</v>
       </c>
@@ -43243,7 +43517,7 @@
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G50" s="434"/>
+      <c r="G50" s="432"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43257,7 +43531,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44016,7 +44290,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="460"/>
+      <c r="F22" s="458"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
@@ -44162,19 +44436,19 @@
         <f>F3/'PRIHODKI IN STROŠKI'!F6</f>
         <v>1.1216062214670557E-3</v>
       </c>
-      <c r="G30" s="462">
+      <c r="G30" s="460">
         <v>0</v>
       </c>
-      <c r="H30" s="462">
+      <c r="H30" s="460">
         <v>0</v>
       </c>
-      <c r="I30" s="462">
+      <c r="I30" s="460">
         <v>0</v>
       </c>
-      <c r="J30" s="462">
+      <c r="J30" s="460">
         <v>0</v>
       </c>
-      <c r="K30" s="462">
+      <c r="K30" s="460">
         <v>0</v>
       </c>
     </row>
@@ -44572,10 +44846,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23540F03-C83E-4C68-8BB8-3F847A129C1D}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45295,28 +45569,75 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="90" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="B25" s="419">
+      <c r="B25" s="7">
         <v>23009989</v>
       </c>
-      <c r="C25" s="419">
+      <c r="C25" s="7">
         <v>28584812</v>
       </c>
-      <c r="D25" s="419">
+      <c r="D25" s="7">
         <v>36268092</v>
       </c>
-      <c r="E25" s="419">
+      <c r="E25" s="7">
         <v>45510666</v>
       </c>
-      <c r="F25" s="420">
+      <c r="F25" s="563">
         <v>55347711</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F26" s="29"/>
+      <c r="A26" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="561">
+        <f>(B3+B6)/(B3+B6+B25)</f>
+        <v>0.36845559048126808</v>
+      </c>
+      <c r="C26" s="561">
+        <f t="shared" ref="C26:F26" si="2">(C3+C6)/(C3+C6+C25)</f>
+        <v>0.29424347266592055</v>
+      </c>
+      <c r="D26" s="561">
+        <f t="shared" si="2"/>
+        <v>0.20101646098422238</v>
+      </c>
+      <c r="E26" s="561">
+        <f t="shared" si="2"/>
+        <v>0.27749450381553842</v>
+      </c>
+      <c r="F26" s="561">
+        <f t="shared" si="2"/>
+        <v>0.26527884955777115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="93" t="s">
+        <v>329</v>
+      </c>
+      <c r="B27" s="562">
+        <f>B25/(B25+B3+B6)</f>
+        <v>0.63154440951873192</v>
+      </c>
+      <c r="C27" s="562">
+        <f t="shared" ref="C27:F27" si="3">C25/(C25+C3+C6)</f>
+        <v>0.70575652733407945</v>
+      </c>
+      <c r="D27" s="562">
+        <f t="shared" si="3"/>
+        <v>0.79898353901577757</v>
+      </c>
+      <c r="E27" s="562">
+        <f t="shared" si="3"/>
+        <v>0.72250549618446158</v>
+      </c>
+      <c r="F27" s="562">
+        <f t="shared" si="3"/>
+        <v>0.73472115044222885</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dodane študije - povzetki in končni odbitek
</commit_message>
<xml_diff>
--- a/Diploma podatki/ANALIZA_POSLOVANJA.xlsx
+++ b/Diploma podatki/ANALIZA_POSLOVANJA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neža\Documents\GitHub\Diplomska-naloga-\Diploma podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A2F5BE-F0C9-4AC1-BE63-40E5F1560B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914AC70-ADDB-47A5-A6FC-91B3DDF1C037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{0DAC0375-5244-478E-9483-C7B8579F68F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{0DAC0375-5244-478E-9483-C7B8579F68F1}"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDA" sheetId="7" r:id="rId1"/>
@@ -342,6 +342,30 @@
     <author>Neža</author>
   </authors>
   <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{DC6C5F55-943D-48AB-A485-9CFB8CE57658}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neža:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.sec.gov/Archives/edgar/data/48272/000104746904029419/a2143709zex-99_c2.htm</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D23" authorId="0" shapeId="0" xr:uid="{1C00D69D-CE6F-48BC-AAD7-D03EDD8DF1E7}">
       <text>
         <r>
@@ -363,6 +387,30 @@
           </rPr>
           <t xml:space="preserve">
 https://www.abi.org/abi-journal/update-on-study-of-discount-for-lack-of-marketability#1a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{A2518D1A-B261-47A9-95D5-BB3FE1430D26}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neža:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+http://www.philipsaunders.com/TheFirm/Publications/MarketabilityDiscounts/tabid/97/Default.aspx</t>
         </r>
       </text>
     </comment>
@@ -417,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A65" authorId="0" shapeId="0" xr:uid="{D93067B5-77D5-45F7-B909-4ECD138D8379}">
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{D93067B5-77D5-45F7-B909-4ECD138D8379}">
       <text>
         <r>
           <rPr>
@@ -442,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A87" authorId="0" shapeId="0" xr:uid="{DEB82F84-5463-44C8-B506-5E497DE8D0BF}">
+    <comment ref="A82" authorId="0" shapeId="0" xr:uid="{DEB82F84-5463-44C8-B506-5E497DE8D0BF}">
       <text>
         <r>
           <rPr>
@@ -1024,7 +1072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="433">
   <si>
     <t>opredmetena osnovna</t>
   </si>
@@ -2109,22 +2157,10 @@
     <t>Zajetih 72 transakcij v letih 1991 - 1995</t>
   </si>
   <si>
-    <t>Preučevanih 115 zasebnih transakcij, vključeno z lastnimi delnicami večjih industrijskih korporacij. Večina se jih je prodajala z diskontom, nekaj pa tudi s premijo ali kar točno po tržni ceni.  Da bi dobili bolj objektivne rezultate so naknadno izključili vse transakcije podjetij z manj kot 3 milijoni prihodkov.</t>
-  </si>
-  <si>
-    <t>Analiziranih preko 100 transakcij - rezultat potrjuje, da je odbitek močno povezan z višino prihodkov podjetja.</t>
-  </si>
-  <si>
-    <t>Preučevanih 44 zasebnih transakcij - z rezultati si lahko razlagajo le 67 odstotkov odbitkov, raziskava ni dosegla željenih rezultatov</t>
-  </si>
-  <si>
     <t>Preučevanih 28 transakcij</t>
   </si>
   <si>
     <t>Preučevanih 33 transakcij</t>
-  </si>
-  <si>
-    <t>Preučevanih 69 transakcij</t>
   </si>
   <si>
     <t>Preučevanih 146 transakcij desetih večjih korporacij</t>
@@ -2229,9 +2265,6 @@
     <t xml:space="preserve">po statutu vsak delničar mora za prodajo delnice osebi zunaj obstoječega kroga delničarjev pridobiti soglasje s strani uprave. </t>
   </si>
   <si>
-    <t>ni posebej relevantno</t>
-  </si>
-  <si>
     <t>vodstvo se je nedolgo nazaj zamenjalo, a stremi k podobnim ciljem</t>
   </si>
   <si>
@@ -2274,16 +2307,7 @@
     <t>prodaja se ena delnica</t>
   </si>
   <si>
-    <t>(-) večji diskont povzročajo večja količina delnic v prodaji (v paketu), nižji zaslužki podjetja in nižja prodaja, nižja tržna vrednost podjetja, količina restriktivnih delnic znotraj vseh izdanih delnic podjetja</t>
-  </si>
-  <si>
     <t>Raziskave restriktivnih delnic od začetka niso upoštevale, da lahko diskont pri vrednosti restriktivne delnice povzroča tudi kompenzacija za investitorja za v prihodnosti predvidene storitve podjetju, ne pa izključno pomanjkljivost tržljivosti.</t>
-  </si>
-  <si>
-    <t>volatilnost cene delnice</t>
-  </si>
-  <si>
-    <t>velikost podjetja</t>
   </si>
   <si>
     <t>raznolikost produktov</t>
@@ -2292,22 +2316,7 @@
     <t>geografska razpršenost trga</t>
   </si>
   <si>
-    <t>odvisnost od dobaviteljev</t>
-  </si>
-  <si>
-    <t>odvisnost od strank</t>
-  </si>
-  <si>
-    <t>prelaganje izdatkov</t>
-  </si>
-  <si>
-    <t>Ker pre IPO raziskave vključujejo le uspešna podjetja, za katera je znano, da bodo v prihodnosti postala javna, je odbitek pri teh raziskavah prevelik, oziroma je prevelik pomen nižje vrednosti pred prvo javno ponudbo posvečen pomanjkanju tržljivosti. Na večjo razliko namreč vplivajo tudi drugi dejavniki. Zato sem pri svojem ocenjevanju izhajala iz spodnjih mej odbitkov, ugotovljenih pri teh raziskavah. Če pri tem posebej izpostavim WMA študijo (zadnjo narejeno, za leta 1988-2000), ta izključuje vse transakcije z osebami, ki so na sumljiv način povezane z vodstvom in drugimi koristi v podjetjih, zato sem znotraj preIPO študij to vzela za najbolj relevantno.</t>
-  </si>
-  <si>
     <t>POVZETKI:</t>
-  </si>
-  <si>
-    <t>Pri ocenjevanju torej izhajam iz bolj relevantnih ocen za odbitke, torej ocene po pre IPO študijah. Te v povprečju določajo 45% odbitek, pri čemer pa sem sama v začetku izhajala iz raziskave WMA, ki je po moji oceni najbolj relevantna in za naše podjetje najprimernejša. Za izhodišče sem vzela spodnji del ugotovljenih odbitkov te raziskave (35%). Glede na navedenih 10 faktorjev, ki naj bi bili najbolj relevantni pri vplivu na spreminjanje odbitka glede na posebne lastnosti podjetij, bi našemu podjetju pripisala odbitek v višini 32%, saj sta od vseh faktorjev na povečanje odbitka vplivali le omejitev pri prenosu lastništva in predkupna pravica uprave do delnice v prodaji tretji osebi. Vsi ostali faktorji so diskont zniževali.</t>
   </si>
   <si>
     <t>ZAKLJUČEK:</t>
@@ -2327,6 +2336,42 @@
   <si>
     <t>(-) rast prihodkov našemu podjetju, tudi pri napovedih v prihodnosti</t>
   </si>
+  <si>
+    <t>Dokaz, da je odbitek močno povezan z dobo, ko delnice ne moreš prodati - na sredini raziskave se je čas držanja restriktivne delnice zmanjšala za polovico. Ugotovljeni vplivi na odbitek: negativno (večji prihodki, večja vrednost paketa restriktivnih delnic na trgu, večja tržna vrednost podjetja, večji dobiček, večje izplačilo dividend) in pozitivno (večji paket restriktivnih delnic, ki se prodaja, daljše obdobje minimalnega držanja kupljenih delnic).</t>
+  </si>
+  <si>
+    <t>Preučevanih 115 zasebnih transakcij, vključeno z lastnimi delnicami večjih industrijskih korporacij. Večina se jih je prodajala z diskontom, nekaj pa tudi s premijo ali kar točno po tržni ceni.  Da bi dobili bolj objektivne rezultate so naknadno izključili vse transakcije podjetij z manj kot 3 milijoni prihodkov. V nadgradnji raziskave so vključili zasebna podjetja, pri katerih: je razkrito finančno stanje javnosti, se restriktivne delnice po vseh drugih lastnostih (razen tržljivosti) ujemajo z javno tržljivimi, je na voljo dovolj podatkov za analizo, se delnica na odprtem trgu prodaja za vsaj 2 dolarja, podjetje ni v fazi razvoja, ni zaznane finančne izgube v letu pred transakcijo. Ugotovitve: večji odbitek pri manjših podjetjih (glede na prihodek), pri počasneje rastočih podjetjih, pri manjši stabilnosti prihodka, pri podjetjih z manjšo vrednostjo delnice, z manjšo tržno kapitalizacijo, z večjim blokom delnic v prodaji, z daljšim minimalnim obdobjem držanja delnice pred možnostjo prodaje.</t>
+  </si>
+  <si>
+    <t>dejavniki zajeti v spodnjem povzetku</t>
+  </si>
+  <si>
+    <t>Analiziranih preko 100 transakcij - rezultat potrjuje, da je odbitek močno povezan z višino prihodkov podjetja, tržno kapitailzacijo podjetja, velikostjo bloka delnic v prodaji.</t>
+  </si>
+  <si>
+    <t>Preučevanih 44 zasebnih transakcij - z rezultati si lahko razlagajo le 67 odstotkov odbitkov, raziskava ni dosegla željenih rezultatov.</t>
+  </si>
+  <si>
+    <t>Preučevanih 69 transakcij, ugotovitev da večji diskont povzročajo večja količina delnic v prodaji (v paketu), nižji zaslužki podjetja in nižja prodaja, nižja tržna vrednost podjetja, količina restriktivnih delnic znotraj vseh izdanih delnic podjetja.</t>
+  </si>
+  <si>
+    <t>dejavniki obrazloženi v spodnjem povzetku</t>
+  </si>
+  <si>
+    <t>Ker preIPO raziskave vsebujejo transakcije podjetij, ki v prihodnosti uspešno prodrejo na javni trg, so ti odbitki višji, čim večje je tveganje vstopa. Zato pri našem podjetju izhajam iz zgornjih mej ugotovljenih odbitkov, saj o izstopu iz zasebnega lastništva vodstvo ne razmišlja. Če pri tem posebej izpostavim WMA študijo (zadnjo narejeno, za leta 1988-2000), ta izključuje tudi vse transakcije z osebami, ki so na sumljiv način povezane z vodstvom in drugimi koristi v podjetjih, vzete so preIPO cene iz do treh let pred prvo javno ponudbo, zato sem to raziskavo vzela za najbolj relevantno.</t>
+  </si>
+  <si>
+    <t>Pri ocenjevanju torej izhajam iz bolj relevantnih ocen za odbitke, torej ocene po pre IPO študijah. Te v povprečju določajo 45% odbitek, pri čemer pa sem sama v začetku izhajala iz raziskave WMA, ki je po moji oceni najbolj relevantna in za naše podjetje najprimernejša. Za izhodišče sem vzela zgornji del ugotovljenih odbitkov te raziskave, kot opisano v povzetkih (49%). Glede na navedenih 10 faktorjev, ki naj bi bili najbolj relevantni pri vplivu na spreminjanje odbitka glede na posebne lastnosti podjetij, bi našemu podjetju pripisala odbitek v višini 40%, saj sta od vseh faktorjev na povečanje odbitka vplivali le omejitev pri prenosu lastništva in predkupna pravica uprave do delnice v prodaji tretji osebi. Vsi ostali faktorji so diskont zniževali.</t>
+  </si>
+  <si>
+    <t>http://www.philipsaunders.com/TheFirm/Publications/MarketabilityDiscounts/tabid/97/Default.aspx</t>
+  </si>
+  <si>
+    <t>širjenje proizvodnje, novi trgi in proizvodi</t>
+  </si>
+  <si>
+    <t>tuj trg, podružnica na Kitajskem, možnost širjenja</t>
+  </si>
 </sst>
 </file>
 
@@ -2344,7 +2389,7 @@
     <numFmt numFmtId="169" formatCode="_-* #,##0.000\ &quot;€&quot;_-;\-* #,##0.000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2552,16 +2597,8 @@
       <charset val="238"/>
       <scheme val="major"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2643,6 +2680,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3517,7 +3560,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="657">
+  <cellXfs count="666">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -4113,15 +4156,8 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4144,11 +4180,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4167,50 +4215,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4231,20 +4236,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hiperpovezava" xfId="9" builtinId="8"/>
@@ -42254,10 +42326,10 @@
     </row>
     <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="631" t="s">
+      <c r="A88" s="644" t="s">
         <v>298</v>
       </c>
-      <c r="B88" s="632"/>
+      <c r="B88" s="645"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="55" t="s">
@@ -43075,7 +43147,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43097,7 +43169,7 @@
         <v>256</v>
       </c>
       <c r="F2" s="434" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G2" s="476" t="s">
         <v>254</v>
@@ -43157,25 +43229,25 @@
         <v>11421674</v>
       </c>
       <c r="L3" s="515" t="s">
-        <v>374</v>
-      </c>
-      <c r="M3" s="606">
+        <v>370</v>
+      </c>
+      <c r="M3" s="599">
         <f>PASIVA!B3+PASIVA!B6</f>
         <v>13424486</v>
       </c>
-      <c r="N3" s="606">
+      <c r="N3" s="599">
         <f>PASIVA!C3+PASIVA!C6</f>
         <v>11917558</v>
       </c>
-      <c r="O3" s="606">
+      <c r="O3" s="599">
         <f>PASIVA!D3+PASIVA!D6</f>
         <v>9124698</v>
       </c>
-      <c r="P3" s="606">
+      <c r="P3" s="599">
         <f>PASIVA!E3+PASIVA!E6</f>
         <v>17479396</v>
       </c>
-      <c r="Q3" s="607">
+      <c r="Q3" s="600">
         <f>PASIVA!F3+PASIVA!F6</f>
         <v>19983877</v>
       </c>
@@ -43193,16 +43265,16 @@
         <v>0.19</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G4" s="453" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="H4" s="453"/>
       <c r="I4" s="453"/>
       <c r="J4" s="54"/>
       <c r="L4" s="515" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="M4" s="135">
         <v>184191</v>
@@ -43210,7 +43282,7 @@
       <c r="N4" s="135">
         <v>278847</v>
       </c>
-      <c r="O4" s="608">
+      <c r="O4" s="601">
         <v>475197</v>
       </c>
       <c r="P4" s="135">
@@ -43231,7 +43303,7 @@
         <f>C3*(1-D4)</f>
         <v>1.4767391232442036E-2</v>
       </c>
-      <c r="D5" s="605">
+      <c r="D5" s="598">
         <f>3.6%</f>
         <v>3.6000000000000004E-2</v>
       </c>
@@ -43246,23 +43318,23 @@
       <c r="I5" s="454"/>
       <c r="J5" s="94"/>
       <c r="L5" s="516"/>
-      <c r="M5" s="609">
+      <c r="M5" s="602">
         <f>M4/M3</f>
         <v>1.3720525314712236E-2</v>
       </c>
-      <c r="N5" s="609">
+      <c r="N5" s="602">
         <f t="shared" ref="N5:Q5" si="0">N4/N3</f>
         <v>2.3397998146935807E-2</v>
       </c>
-      <c r="O5" s="609">
+      <c r="O5" s="602">
         <f t="shared" si="0"/>
         <v>5.2078107132970321E-2</v>
       </c>
-      <c r="P5" s="609">
+      <c r="P5" s="602">
         <f t="shared" si="0"/>
         <v>1.8865697647676156E-2</v>
       </c>
-      <c r="Q5" s="610">
+      <c r="Q5" s="603">
         <f t="shared" si="0"/>
         <v>1.8231347200545721E-2</v>
       </c>
@@ -43341,11 +43413,11 @@
       <c r="C12" s="473">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="F12" s="623" t="s">
+      <c r="F12" s="620" t="s">
         <v>270</v>
       </c>
-      <c r="G12" s="624"/>
-      <c r="H12" s="625"/>
+      <c r="G12" s="621"/>
+      <c r="H12" s="622"/>
       <c r="J12" s="497" t="s">
         <v>284</v>
       </c>
@@ -43403,18 +43475,18 @@
       <c r="G15" s="171">
         <v>1.03E-2</v>
       </c>
-      <c r="J15" s="623" t="s">
+      <c r="J15" s="620" t="s">
         <v>291</v>
       </c>
-      <c r="K15" s="624"/>
-      <c r="L15" s="624"/>
-      <c r="M15" s="625"/>
+      <c r="K15" s="621"/>
+      <c r="L15" s="621"/>
+      <c r="M15" s="622"/>
     </row>
     <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="464" t="s">
         <v>250</v>
       </c>
-      <c r="C16" s="622"/>
+      <c r="C16" s="612"/>
       <c r="F16" s="481">
         <v>42826</v>
       </c>
@@ -43512,11 +43584,11 @@
       <c r="G25" s="501"/>
     </row>
     <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="626" t="s">
+      <c r="F26" s="623" t="s">
         <v>283</v>
       </c>
-      <c r="G26" s="627"/>
-      <c r="H26" s="628"/>
+      <c r="G26" s="624"/>
+      <c r="H26" s="625"/>
     </row>
     <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F27" s="502">
@@ -43699,10 +43771,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFF3F75-511C-494C-979E-3E00983A6C23}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A65" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43725,71 +43797,71 @@
       <c r="E2" s="594"/>
     </row>
     <row r="3" spans="1:5" s="429" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="595" t="s">
+      <c r="A3" s="654" t="s">
         <v>335</v>
       </c>
-      <c r="B3" s="596" t="s">
+      <c r="B3" s="655" t="s">
         <v>336</v>
       </c>
-      <c r="C3" s="468"/>
-      <c r="D3" s="468"/>
-      <c r="E3" s="597"/>
+      <c r="C3" s="656"/>
+      <c r="D3" s="657"/>
+      <c r="E3" s="658"/>
     </row>
     <row r="4" spans="1:5" s="429" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="598"/>
-      <c r="B4" s="596" t="s">
+      <c r="A4" s="659"/>
+      <c r="B4" s="655" t="s">
         <v>339</v>
       </c>
-      <c r="C4" s="596" t="s">
+      <c r="C4" s="655" t="s">
         <v>340</v>
       </c>
-      <c r="D4" s="596" t="s">
+      <c r="D4" s="660" t="s">
         <v>341</v>
       </c>
-      <c r="E4" s="599" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="429" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="598">
+      <c r="E4" s="661" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="429" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="595">
         <v>1</v>
       </c>
-      <c r="B5" s="601" t="s">
+      <c r="B5" s="647" t="s">
         <v>345</v>
       </c>
-      <c r="C5" s="600" t="s">
+      <c r="C5" s="648" t="s">
         <v>357</v>
       </c>
-      <c r="D5" s="615" t="s">
-        <v>358</v>
-      </c>
-      <c r="E5" s="655" t="s">
-        <v>432</v>
+      <c r="D5" s="608" t="s">
+        <v>421</v>
+      </c>
+      <c r="E5" s="626" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="515">
         <v>2</v>
       </c>
-      <c r="B6" s="603" t="s">
+      <c r="B6" s="649" t="s">
         <v>346</v>
       </c>
-      <c r="C6" s="600" t="s">
+      <c r="C6" s="648" t="s">
         <v>359</v>
       </c>
-      <c r="D6" s="615" t="s">
+      <c r="D6" s="608" t="s">
         <v>358</v>
       </c>
-      <c r="E6" s="655"/>
+      <c r="E6" s="626"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="598">
+      <c r="A7" s="595">
         <v>3</v>
       </c>
-      <c r="B7" s="603" t="s">
+      <c r="B7" s="649" t="s">
         <v>347</v>
       </c>
-      <c r="C7" s="135">
+      <c r="C7" s="650">
         <v>20</v>
       </c>
       <c r="D7" s="135" t="s">
@@ -43797,65 +43869,67 @@
       </c>
       <c r="E7" s="220"/>
     </row>
-    <row r="8" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A8" s="515">
         <v>4</v>
       </c>
-      <c r="B8" s="603" t="s">
+      <c r="B8" s="649" t="s">
         <v>348</v>
       </c>
-      <c r="C8" s="135">
+      <c r="C8" s="650">
         <v>26</v>
       </c>
-      <c r="D8" s="616" t="s">
-        <v>361</v>
-      </c>
-      <c r="E8" s="604"/>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="598">
+      <c r="D8" s="609" t="s">
+        <v>422</v>
+      </c>
+      <c r="E8" s="619" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="595">
         <v>5</v>
       </c>
-      <c r="B9" s="603" t="s">
+      <c r="B9" s="649" t="s">
         <v>349</v>
       </c>
-      <c r="C9" s="468">
+      <c r="C9" s="646">
         <v>23</v>
       </c>
-      <c r="D9" s="616" t="s">
-        <v>362</v>
-      </c>
-      <c r="E9" s="656" t="s">
-        <v>433</v>
+      <c r="D9" s="609" t="s">
+        <v>424</v>
+      </c>
+      <c r="E9" s="619" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="515">
         <v>6</v>
       </c>
-      <c r="B10" s="603" t="s">
+      <c r="B10" s="649" t="s">
         <v>350</v>
       </c>
-      <c r="C10" s="468">
+      <c r="C10" s="646">
         <v>24</v>
       </c>
-      <c r="D10" s="616" t="s">
-        <v>363</v>
-      </c>
-      <c r="E10" s="654"/>
+      <c r="D10" s="609" t="s">
+        <v>425</v>
+      </c>
+      <c r="E10" s="618"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="598">
+      <c r="A11" s="595">
         <v>7</v>
       </c>
-      <c r="B11" s="603" t="s">
+      <c r="B11" s="649" t="s">
         <v>351</v>
       </c>
-      <c r="C11" s="468">
+      <c r="C11" s="646">
         <v>45</v>
       </c>
       <c r="D11" s="135" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E11" s="220"/>
     </row>
@@ -43863,93 +43937,93 @@
       <c r="A12" s="515">
         <v>8</v>
       </c>
-      <c r="B12" s="602" t="s">
+      <c r="B12" s="651" t="s">
         <v>337</v>
       </c>
-      <c r="C12" s="468">
+      <c r="C12" s="646">
         <v>31</v>
       </c>
       <c r="D12" s="135" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E12" s="220"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="598">
+      <c r="A13" s="595">
         <v>9</v>
       </c>
-      <c r="B13" s="602" t="s">
+      <c r="B13" s="651" t="s">
         <v>338</v>
       </c>
-      <c r="C13" s="468">
+      <c r="C13" s="646">
         <v>34</v>
       </c>
       <c r="D13" s="135" t="s">
-        <v>366</v>
-      </c>
-      <c r="E13" s="641" t="s">
-        <v>416</v>
+        <v>426</v>
+      </c>
+      <c r="E13" s="615" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="515">
         <v>10</v>
       </c>
-      <c r="B14" s="603" t="s">
+      <c r="B14" s="649" t="s">
         <v>352</v>
       </c>
-      <c r="C14" s="468">
+      <c r="C14" s="646">
         <v>33</v>
       </c>
       <c r="D14" s="135" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E14" s="220"/>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="598">
+      <c r="A15" s="595">
         <v>11</v>
       </c>
-      <c r="B15" s="603" t="s">
+      <c r="B15" s="649" t="s">
         <v>355</v>
       </c>
-      <c r="C15" s="468">
+      <c r="C15" s="646">
         <v>24</v>
       </c>
-      <c r="D15" s="616" t="s">
-        <v>431</v>
-      </c>
-      <c r="E15" s="656" t="s">
-        <v>430</v>
+      <c r="D15" s="609" t="s">
+        <v>418</v>
+      </c>
+      <c r="E15" s="619" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="515">
         <v>12</v>
       </c>
-      <c r="B16" s="603" t="s">
+      <c r="B16" s="649" t="s">
         <v>356</v>
       </c>
-      <c r="C16" s="468">
+      <c r="C16" s="646">
         <v>33</v>
       </c>
       <c r="D16" s="135" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E16" s="220"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="598">
+      <c r="A17" s="595">
         <v>13</v>
       </c>
-      <c r="B17" s="603" t="s">
+      <c r="B17" s="649" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="468">
+      <c r="C17" s="646">
         <v>34</v>
       </c>
       <c r="D17" s="135" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E17" s="220"/>
     </row>
@@ -43957,550 +44031,517 @@
       <c r="A18" s="515">
         <v>14</v>
       </c>
-      <c r="B18" s="603" t="s">
+      <c r="B18" s="649" t="s">
         <v>354</v>
       </c>
-      <c r="C18" s="468">
+      <c r="C18" s="646">
         <v>35</v>
       </c>
       <c r="D18" s="135" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E18" s="220"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="564" t="s">
+      <c r="A19" s="654" t="s">
         <v>342</v>
       </c>
-      <c r="B19" s="218" t="s">
+      <c r="B19" s="655" t="s">
         <v>343</v>
       </c>
-      <c r="C19" s="135"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="220"/>
+      <c r="C19" s="656"/>
+      <c r="D19" s="657"/>
+      <c r="E19" s="658"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="515"/>
-      <c r="B20" s="218" t="s">
+      <c r="A20" s="659"/>
+      <c r="B20" s="655" t="s">
         <v>339</v>
       </c>
-      <c r="C20" s="218" t="s">
+      <c r="C20" s="655" t="s">
         <v>340</v>
       </c>
-      <c r="D20" s="218" t="s">
+      <c r="D20" s="660" t="s">
         <v>341</v>
       </c>
-      <c r="E20" s="219"/>
+      <c r="E20" s="661"/>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="515">
         <v>1</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="650" t="s">
         <v>344</v>
       </c>
-      <c r="C21" s="468" t="s">
-        <v>376</v>
-      </c>
-      <c r="D21" s="616" t="s">
-        <v>377</v>
-      </c>
-      <c r="E21" s="604"/>
+      <c r="C21" s="646" t="s">
+        <v>372</v>
+      </c>
+      <c r="D21" s="609" t="s">
+        <v>373</v>
+      </c>
+      <c r="E21" s="597"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="515">
         <v>2</v>
       </c>
-      <c r="B22" s="135" t="s">
-        <v>378</v>
-      </c>
-      <c r="C22" s="618">
+      <c r="B22" s="650" t="s">
+        <v>374</v>
+      </c>
+      <c r="C22" s="652">
         <v>0.52</v>
       </c>
-      <c r="D22" s="616"/>
-      <c r="E22" s="604"/>
+      <c r="D22" s="609"/>
+      <c r="E22" s="597"/>
     </row>
     <row r="23" spans="1:5" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="516">
         <v>3</v>
       </c>
-      <c r="B23" s="517" t="s">
+      <c r="B23" s="653" t="s">
         <v>337</v>
       </c>
-      <c r="C23" s="517" t="s">
-        <v>381</v>
-      </c>
-      <c r="D23" s="617" t="s">
-        <v>380</v>
-      </c>
-      <c r="E23" s="653" t="s">
-        <v>429</v>
+      <c r="C23" s="653" t="s">
+        <v>377</v>
+      </c>
+      <c r="D23" s="610" t="s">
+        <v>376</v>
+      </c>
+      <c r="E23" s="662" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="652" t="s">
-        <v>426</v>
+      <c r="B27" s="617" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="645" t="s">
-        <v>379</v>
-      </c>
-      <c r="C29" s="648" t="s">
-        <v>417</v>
-      </c>
-      <c r="D29" s="648" t="s">
-        <v>425</v>
-      </c>
-      <c r="E29" s="648" t="s">
-        <v>382</v>
+      <c r="B29" s="627" t="s">
+        <v>375</v>
+      </c>
+      <c r="C29" s="630" t="s">
+        <v>411</v>
+      </c>
+      <c r="D29" s="630" t="s">
+        <v>428</v>
+      </c>
+      <c r="E29" s="630" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="646"/>
-      <c r="C30" s="649"/>
-      <c r="D30" s="649"/>
-      <c r="E30" s="649"/>
+      <c r="B30" s="628"/>
+      <c r="C30" s="631"/>
+      <c r="D30" s="631"/>
+      <c r="E30" s="631"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="646"/>
-      <c r="C31" s="649"/>
-      <c r="D31" s="649"/>
-      <c r="E31" s="649"/>
+      <c r="B31" s="628"/>
+      <c r="C31" s="631"/>
+      <c r="D31" s="631"/>
+      <c r="E31" s="631"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="646"/>
-      <c r="C32" s="649"/>
-      <c r="D32" s="649"/>
-      <c r="E32" s="649"/>
+      <c r="B32" s="628"/>
+      <c r="C32" s="631"/>
+      <c r="D32" s="631"/>
+      <c r="E32" s="631"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="646"/>
-      <c r="C33" s="649"/>
-      <c r="D33" s="649"/>
-      <c r="E33" s="649"/>
+      <c r="B33" s="628"/>
+      <c r="C33" s="631"/>
+      <c r="D33" s="631"/>
+      <c r="E33" s="631"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="646"/>
-      <c r="C34" s="649"/>
-      <c r="D34" s="649"/>
-      <c r="E34" s="649"/>
+      <c r="B34" s="628"/>
+      <c r="C34" s="631"/>
+      <c r="D34" s="631"/>
+      <c r="E34" s="631"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="647"/>
-      <c r="C35" s="650"/>
-      <c r="D35" s="650"/>
-      <c r="E35" s="650"/>
+      <c r="B35" s="629"/>
+      <c r="C35" s="632"/>
+      <c r="D35" s="632"/>
+      <c r="E35" s="632"/>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="629" t="s">
-        <v>383</v>
-      </c>
-      <c r="B48" s="630"/>
-      <c r="C48" s="630"/>
-      <c r="D48" s="630"/>
-      <c r="E48" s="619"/>
+      <c r="A48" s="633" t="s">
+        <v>379</v>
+      </c>
+      <c r="B48" s="634"/>
+      <c r="C48" s="634"/>
+      <c r="D48" s="634"/>
+      <c r="E48" s="611"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="515"/>
       <c r="B49" s="218" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C49" s="218" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D49" s="218" t="s">
-        <v>396</v>
-      </c>
-      <c r="E49" s="599" t="s">
-        <v>397</v>
+        <v>392</v>
+      </c>
+      <c r="E49" s="596" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="515"/>
       <c r="B50" s="135" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C50" s="135" t="s">
-        <v>387</v>
-      </c>
-      <c r="D50" s="634" t="s">
+        <v>383</v>
+      </c>
+      <c r="D50" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E50" s="220" t="s">
-        <v>398</v>
+      <c r="E50" s="663" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="515"/>
       <c r="B51" s="135" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C51" s="135" t="s">
-        <v>389</v>
-      </c>
-      <c r="D51" s="634" t="s">
+        <v>385</v>
+      </c>
+      <c r="D51" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E51" s="220" t="s">
-        <v>407</v>
+      <c r="E51" s="663" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="515"/>
       <c r="B52" s="468" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C52" s="468" t="s">
-        <v>387</v>
-      </c>
-      <c r="D52" s="634" t="s">
-        <v>399</v>
-      </c>
-      <c r="E52" s="220" t="s">
-        <v>400</v>
+        <v>383</v>
+      </c>
+      <c r="D52" s="613" t="s">
+        <v>395</v>
+      </c>
+      <c r="E52" s="663" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="515"/>
-      <c r="B53" s="620" t="s">
-        <v>391</v>
-      </c>
-      <c r="C53" s="620" t="s">
-        <v>392</v>
-      </c>
-      <c r="D53" s="635"/>
-      <c r="E53" s="621" t="s">
-        <v>401</v>
-      </c>
+      <c r="B53" s="664" t="s">
+        <v>387</v>
+      </c>
+      <c r="C53" s="664" t="s">
+        <v>388</v>
+      </c>
+      <c r="D53" s="614"/>
+      <c r="E53" s="665"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="515"/>
       <c r="B54" s="468" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C54" s="468" t="s">
-        <v>387</v>
-      </c>
-      <c r="D54" s="634" t="s">
+        <v>383</v>
+      </c>
+      <c r="D54" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E54" s="220" t="s">
-        <v>406</v>
+      <c r="E54" s="663" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="515"/>
       <c r="B55" s="468" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C55" s="468" t="s">
-        <v>389</v>
-      </c>
-      <c r="D55" s="634" t="s">
+        <v>385</v>
+      </c>
+      <c r="D55" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E55" s="220" t="s">
-        <v>402</v>
+      <c r="E55" s="663" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="515"/>
       <c r="B56" s="468" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C56" s="468" t="s">
-        <v>392</v>
-      </c>
-      <c r="D56" s="634" t="s">
+        <v>388</v>
+      </c>
+      <c r="D56" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E56" s="220" t="s">
-        <v>404</v>
+      <c r="E56" s="663" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="515"/>
       <c r="B57" s="468" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C57" s="468" t="s">
-        <v>387</v>
-      </c>
-      <c r="D57" s="634" t="s">
+        <v>383</v>
+      </c>
+      <c r="D57" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E57" s="220" t="s">
-        <v>408</v>
+      <c r="E57" s="663" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="515"/>
       <c r="B58" s="468" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C58" s="468" t="s">
-        <v>387</v>
-      </c>
-      <c r="D58" s="634" t="s">
-        <v>399</v>
-      </c>
-      <c r="E58" s="220" t="s">
-        <v>409</v>
+        <v>383</v>
+      </c>
+      <c r="D58" s="613" t="s">
+        <v>395</v>
+      </c>
+      <c r="E58" s="663" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="515"/>
       <c r="B59" s="468" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C59" s="468" t="s">
-        <v>389</v>
-      </c>
-      <c r="D59" s="634" t="s">
-        <v>399</v>
-      </c>
-      <c r="E59" s="220" t="s">
-        <v>413</v>
+        <v>385</v>
+      </c>
+      <c r="D59" s="613" t="s">
+        <v>395</v>
+      </c>
+      <c r="E59" s="663" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="515"/>
       <c r="B60" s="468"/>
       <c r="C60" s="468"/>
-      <c r="D60" s="634"/>
-      <c r="E60" s="220"/>
+      <c r="D60" s="613"/>
+      <c r="E60" s="663"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="515"/>
       <c r="B61" s="468" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C61" s="468"/>
-      <c r="D61" s="634" t="s">
+      <c r="D61" s="613" t="s">
         <v>278</v>
       </c>
-      <c r="E61" s="220" t="s">
-        <v>415</v>
+      <c r="E61" s="663" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="515"/>
-      <c r="B62" s="468" t="s">
-        <v>418</v>
-      </c>
+      <c r="B62" s="468"/>
       <c r="C62" s="468"/>
-      <c r="D62" s="634"/>
-      <c r="E62" s="220"/>
+      <c r="D62" s="613"/>
+      <c r="E62" s="663"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="515"/>
       <c r="B63" s="468" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C63" s="468"/>
-      <c r="D63" s="634"/>
-      <c r="E63" s="220"/>
+      <c r="D63" s="613" t="s">
+        <v>278</v>
+      </c>
+      <c r="E63" s="663" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="515"/>
-      <c r="B64" s="468"/>
+      <c r="B64" s="468" t="s">
+        <v>413</v>
+      </c>
       <c r="C64" s="468"/>
-      <c r="D64" s="634"/>
-      <c r="E64" s="220"/>
+      <c r="D64" s="613" t="s">
+        <v>278</v>
+      </c>
+      <c r="E64" s="663" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="515"/>
-      <c r="B65" s="468" t="s">
-        <v>420</v>
-      </c>
+      <c r="B65" s="468"/>
       <c r="C65" s="468"/>
-      <c r="D65" s="634"/>
-      <c r="E65" s="220"/>
+      <c r="D65" s="613"/>
+      <c r="E65" s="663"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="515"/>
-      <c r="B66" s="468" t="s">
-        <v>421</v>
-      </c>
+      <c r="B66" s="468"/>
       <c r="C66" s="468"/>
-      <c r="D66" s="634"/>
-      <c r="E66" s="220"/>
+      <c r="D66" s="613"/>
+      <c r="E66" s="663"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="515"/>
-      <c r="B67" s="468" t="s">
-        <v>422</v>
-      </c>
+      <c r="B67" s="468"/>
       <c r="C67" s="468"/>
-      <c r="D67" s="634"/>
-      <c r="E67" s="220"/>
+      <c r="D67" s="613"/>
+      <c r="E67" s="663"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="515"/>
-      <c r="B68" s="468" t="s">
-        <v>423</v>
-      </c>
+      <c r="B68" s="468"/>
       <c r="C68" s="468"/>
-      <c r="D68" s="634"/>
-      <c r="E68" s="220"/>
+      <c r="D68" s="613"/>
+      <c r="E68" s="663"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="515"/>
-      <c r="B69" s="468" t="s">
-        <v>424</v>
-      </c>
+      <c r="B69" s="468"/>
       <c r="C69" s="468"/>
-      <c r="D69" s="634"/>
-      <c r="E69" s="220"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D69" s="613"/>
+      <c r="E69" s="663"/>
+    </row>
+    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="515"/>
-      <c r="B70" s="468"/>
-      <c r="C70" s="468"/>
-      <c r="D70" s="634"/>
+      <c r="B70" s="616" t="s">
+        <v>415</v>
+      </c>
+      <c r="C70" s="135"/>
+      <c r="D70" s="135"/>
       <c r="E70" s="220"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="515"/>
-      <c r="B71" s="468"/>
-      <c r="C71" s="468"/>
-      <c r="D71" s="634"/>
-      <c r="E71" s="220"/>
+      <c r="B71" s="635" t="s">
+        <v>429</v>
+      </c>
+      <c r="C71" s="638"/>
+      <c r="D71" s="640"/>
+      <c r="E71" s="642"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="515"/>
-      <c r="B72" s="468"/>
-      <c r="C72" s="468"/>
-      <c r="D72" s="634"/>
-      <c r="E72" s="220"/>
+      <c r="B72" s="636"/>
+      <c r="C72" s="638"/>
+      <c r="D72" s="640"/>
+      <c r="E72" s="642"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="515"/>
-      <c r="B73" s="468"/>
-      <c r="C73" s="468"/>
-      <c r="D73" s="634"/>
-      <c r="E73" s="220"/>
+      <c r="B73" s="636"/>
+      <c r="C73" s="638"/>
+      <c r="D73" s="640"/>
+      <c r="E73" s="642"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="515"/>
-      <c r="B74" s="468"/>
-      <c r="C74" s="468"/>
-      <c r="D74" s="634"/>
-      <c r="E74" s="220"/>
-    </row>
-    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="636"/>
+      <c r="C74" s="638"/>
+      <c r="D74" s="640"/>
+      <c r="E74" s="642"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="515"/>
-      <c r="B75" s="651" t="s">
-        <v>428</v>
-      </c>
-      <c r="C75" s="135"/>
-      <c r="D75" s="135"/>
-      <c r="E75" s="220"/>
+      <c r="B75" s="636"/>
+      <c r="C75" s="638"/>
+      <c r="D75" s="640"/>
+      <c r="E75" s="642"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="515"/>
-      <c r="B76" s="638" t="s">
-        <v>427</v>
-      </c>
-      <c r="C76" s="643"/>
-      <c r="D76" s="633"/>
-      <c r="E76" s="636"/>
+      <c r="B76" s="636"/>
+      <c r="C76" s="638"/>
+      <c r="D76" s="640"/>
+      <c r="E76" s="642"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="515"/>
-      <c r="B77" s="639"/>
-      <c r="C77" s="643"/>
-      <c r="D77" s="633"/>
-      <c r="E77" s="636"/>
+      <c r="B77" s="636"/>
+      <c r="C77" s="638"/>
+      <c r="D77" s="640"/>
+      <c r="E77" s="642"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="515"/>
-      <c r="B78" s="639"/>
-      <c r="C78" s="643"/>
-      <c r="D78" s="633"/>
-      <c r="E78" s="636"/>
+      <c r="B78" s="636"/>
+      <c r="C78" s="638"/>
+      <c r="D78" s="640"/>
+      <c r="E78" s="642"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="515"/>
-      <c r="B79" s="639"/>
-      <c r="C79" s="643"/>
-      <c r="D79" s="633"/>
-      <c r="E79" s="636"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="515"/>
-      <c r="B80" s="639"/>
-      <c r="C80" s="643"/>
-      <c r="D80" s="633"/>
-      <c r="E80" s="636"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="515"/>
-      <c r="B81" s="639"/>
-      <c r="C81" s="643"/>
-      <c r="D81" s="633"/>
-      <c r="E81" s="636"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="515"/>
-      <c r="B82" s="639"/>
-      <c r="C82" s="643"/>
-      <c r="D82" s="633"/>
-      <c r="E82" s="636"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="515"/>
-      <c r="B83" s="639"/>
-      <c r="C83" s="643"/>
-      <c r="D83" s="633"/>
-      <c r="E83" s="636"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="515"/>
-      <c r="B84" s="639"/>
-      <c r="C84" s="643"/>
-      <c r="D84" s="633"/>
-      <c r="E84" s="636"/>
-    </row>
-    <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="516"/>
-      <c r="B85" s="640"/>
-      <c r="C85" s="644"/>
-      <c r="D85" s="642"/>
-      <c r="E85" s="637"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B87" s="480" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="480" t="s">
-        <v>411</v>
+      <c r="B79" s="636"/>
+      <c r="C79" s="638"/>
+      <c r="D79" s="640"/>
+      <c r="E79" s="642"/>
+    </row>
+    <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="516"/>
+      <c r="B80" s="637"/>
+      <c r="C80" s="639"/>
+      <c r="D80" s="641"/>
+      <c r="E80" s="643"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="480" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="480" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="480" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="B71:B80"/>
+    <mergeCell ref="C71:C80"/>
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="E71:E80"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="B29:B35"/>
     <mergeCell ref="C29:C35"/>
     <mergeCell ref="D29:D35"/>
     <mergeCell ref="E29:E35"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="B76:B85"/>
-    <mergeCell ref="C76:C85"/>
-    <mergeCell ref="D76:D85"/>
-    <mergeCell ref="E76:E85"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B87" r:id="rId1" xr:uid="{9D02BFCE-101F-4872-A0AA-D4924452351B}"/>
-    <hyperlink ref="B88" r:id="rId2" xr:uid="{4C39F3D6-024C-4D38-9577-41321950542F}"/>
+    <hyperlink ref="B82" r:id="rId1" xr:uid="{9D02BFCE-101F-4872-A0AA-D4924452351B}"/>
+    <hyperlink ref="B83" r:id="rId2" xr:uid="{4C39F3D6-024C-4D38-9577-41321950542F}"/>
+    <hyperlink ref="B84" r:id="rId3" xr:uid="{C78ED554-B2C7-45F9-B92A-3E4E3DD6A893}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -44508,8 +44549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F4A1B7-CCDE-4E0D-A100-110DCDF83F93}">
   <dimension ref="B2:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44549,7 +44590,7 @@
       <c r="I3" s="576" t="s">
         <v>315</v>
       </c>
-      <c r="J3" s="611">
+      <c r="J3" s="604">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="K3" s="453">
@@ -44680,18 +44721,18 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="612" t="s">
+      <c r="B13" s="605" t="s">
         <v>332</v>
       </c>
-      <c r="C13" s="613">
+      <c r="C13" s="606">
         <v>0.33400000000000002</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="614" t="s">
+      <c r="B14" s="607" t="s">
         <v>331</v>
       </c>
-      <c r="C14" s="614">
+      <c r="C14" s="607">
         <f>1-(1/(1+C13))</f>
         <v>0.2503748125937032</v>
       </c>
@@ -44701,7 +44742,7 @@
         <v>293</v>
       </c>
       <c r="C15" s="453">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -44710,7 +44751,7 @@
       </c>
       <c r="C17" s="589">
         <f>C10*(1-C15)</f>
-        <v>82.433054326981548</v>
+        <v>79.773923542240198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>